<commit_message>
Updated following the call on 7th Feb.
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Submission" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Inferences" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Genotype" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Haplotype Information" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Tool Settings" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -111,7 +111,25 @@
     <t>sequence_id</t>
   </si>
   <si>
-    <t>closest_IMGT</t>
+    <t>subject_id</t>
+  </si>
+  <si>
+    <t>sequences</t>
+  </si>
+  <si>
+    <t>closest_reference</t>
+  </si>
+  <si>
+    <t>closest_host</t>
+  </si>
+  <si>
+    <t>nt_diff</t>
+  </si>
+  <si>
+    <t>aa_diff</t>
+  </si>
+  <si>
+    <t>cigar</t>
   </si>
   <si>
     <t>unmutated_frequency</t>
@@ -135,12 +153,12 @@
     <t>haplotype_evidence</t>
   </si>
   <si>
-    <t>database_diff</t>
-  </si>
-  <si>
     <t>nt_sequence</t>
   </si>
   <si>
+    <t>phred_score</t>
+  </si>
+  <si>
     <t>repository_name</t>
   </si>
   <si>
@@ -151,13 +169,52 @@
   </si>
   <si>
     <t>Notes on Fields</t>
+  </si>
+  <si>
+    <t>'Number of sequences': where sequences are counted the count
+should be conducted after quality control  UMI processing
+and replicate/error cloud removal.</t>
+  </si>
+  <si>
+    <t>Question for review - should this be the number of distinct
+sequences or a molecule count?</t>
+  </si>
+  <si>
+    <t>'Reference genes and alleles' - this is the set of genes and
+alleles provided to the inference tool.</t>
   </si>
   <si>
     <t>Identifier of the allele, issued by the submitter (need not
 follow any particular format)</t>
   </si>
   <si>
-    <t>The closest known IMGT allele, based on percent identity</t>
+    <t>Identifier of the subject from which this sequence was
+inferred (if inferred from more than one subject, please
+complete separate Inferred_Sequence records for each
+subject)</t>
+  </si>
+  <si>
+    <t>Overall number of sequences assigned to this allele</t>
+  </si>
+  <si>
+    <t>The closest reference gene and allele, based on percent
+identity</t>
+  </si>
+  <si>
+    <t>The closest reference gene and allele that is in the
+subject's inferred genotype, based on percent identity</t>
+  </si>
+  <si>
+    <t>Number of nucleotides that differ between this sequence and
+the closest reference gene and allele</t>
+  </si>
+  <si>
+    <t>Number of amino acids that differ between this sequence and
+the closest reference gene and allele</t>
+  </si>
+  <si>
+    <t>Alignment between this sequence and the closest reference
+gene and allele (CIGAR string)</t>
   </si>
   <si>
     <t>The proportion of records in the sequence dataset matching
@@ -188,10 +245,11 @@
 haplotypes</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>The consensus sequence provided by the inference tool</t>
+  </si>
+  <si>
+    <t>phred string (FASTQ format) for the consensus contig from
+which this nt sequence was inferred</t>
   </si>
   <si>
     <t>Name of the repository in which the sequence has been
@@ -213,12 +271,75 @@
     <t>Notes on FIelds</t>
   </si>
   <si>
+    <t>'Number of sequences': where sequences are counted the count
+should be conducted after quality control UMI processing and
+replicate/error cloud removal.</t>
+  </si>
+  <si>
+    <t>Question for review - should this be the number of distinct
+sequences  or a molecule count?</t>
+  </si>
+  <si>
     <t>Identifier of the allele (either IMGT, or the name assigned
 by the submitter to an inferred gene)</t>
   </si>
   <si>
+    <t>Identifier of the subject from which this genotype was
+inferred (please provide separate genotypes for each
+subject)</t>
+  </si>
+  <si>
+    <t>For inferred alleles, the closest reference gene and allele,
+based on percent identity</t>
+  </si>
+  <si>
+    <t>For inferred alleles, the closest reference gene and allele
+that is in the subject's inferred genotype, based on percent
+identity</t>
+  </si>
+  <si>
+    <t>For inferred alleles, the number of nucleotides that differ
+between this sequence and the closest reference gene and
+allele</t>
+  </si>
+  <si>
+    <t>For inferred alleles, the number of amino acids that differ
+between this sequence and the closest reference gene and
+allele</t>
+  </si>
+  <si>
+    <t>For inferred alleles, the alignment between this sequence
+and the closest reference gene and allele (CIGAR string)</t>
+  </si>
+  <si>
     <t>Is there evidence of differential expression between
 haplotypes?</t>
+  </si>
+  <si>
+    <t>Tool Settings</t>
+  </si>
+  <si>
+    <t>Please provide details of the inference tool, including
+serttings used for this inference.</t>
+  </si>
+  <si>
+    <t>tool_name</t>
+  </si>
+  <si>
+    <t>Name of the inference tool</t>
+  </si>
+  <si>
+    <t>tool_version</t>
+  </si>
+  <si>
+    <t>Version of the inference tool</t>
+  </si>
+  <si>
+    <t>tool_settings</t>
+  </si>
+  <si>
+    <t>Settings/configuration of the tool when used to provide the
+inferences (automatically generated)</t>
   </si>
 </sst>
 </file>
@@ -226,7 +347,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -244,6 +365,14 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <i val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -361,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -381,6 +510,7 @@
     </xf>
     <xf borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -852,7 +982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,25 +991,31 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="3"/>
-    <col customWidth="1" max="2" min="2" width="60"/>
+    <col customWidth="1" max="2" min="2" width="62"/>
     <col customWidth="1" max="3" min="3" width="61"/>
-    <col customWidth="1" max="4" min="4" width="21"/>
-    <col customWidth="1" max="5" min="5" width="21"/>
-    <col customWidth="1" max="6" min="6" width="15"/>
-    <col customWidth="1" max="7" min="7" width="11"/>
-    <col customWidth="1" max="8" min="8" width="11"/>
-    <col customWidth="1" max="9" min="9" width="14"/>
-    <col customWidth="1" max="10" min="10" width="20"/>
-    <col customWidth="1" max="11" min="11" width="15"/>
-    <col customWidth="1" max="12" min="12" width="13"/>
-    <col customWidth="1" max="13" min="13" width="17"/>
-    <col customWidth="1" max="14" min="14" width="15"/>
-    <col customWidth="1" max="15" min="15" width="19"/>
+    <col customWidth="1" max="4" min="4" width="11"/>
+    <col customWidth="1" max="5" min="5" width="19"/>
+    <col customWidth="1" max="6" min="6" width="14"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="9"/>
+    <col customWidth="1" max="9" min="9" width="7"/>
+    <col customWidth="1" max="10" min="10" width="21"/>
+    <col customWidth="1" max="11" min="11" width="21"/>
+    <col customWidth="1" max="12" min="12" width="15"/>
+    <col customWidth="1" max="13" min="13" width="11"/>
+    <col customWidth="1" max="14" min="14" width="11"/>
+    <col customWidth="1" max="15" min="15" width="14"/>
+    <col customWidth="1" max="16" min="16" width="20"/>
+    <col customWidth="1" max="17" min="17" width="13"/>
+    <col customWidth="1" max="18" min="18" width="13"/>
+    <col customWidth="1" max="19" min="19" width="17"/>
+    <col customWidth="1" max="20" min="20" width="15"/>
+    <col customWidth="1" max="21" min="21" width="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15"/>
-    <row r="2" spans="1:15"/>
-    <row r="3" spans="1:15">
+    <row r="1" spans="1:21"/>
+    <row r="2" spans="1:21"/>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -887,16 +1023,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:21">
       <c r="B4" s="1" t="n"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:21">
       <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15"/>
-    <row r="7" spans="1:15">
+    <row r="6" spans="1:21"/>
+    <row r="7" spans="1:21">
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
@@ -936,11 +1072,29 @@
       <c r="N7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="B8" s="6" t="s">
         <v>0</v>
       </c>
@@ -980,11 +1134,29 @@
       <c r="N8" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="O8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="B9" s="6" t="s">
         <v>0</v>
       </c>
@@ -1024,11 +1196,29 @@
       <c r="N9" t="s">
         <v>0</v>
       </c>
-      <c r="O9" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="O9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="B10" s="6" t="s">
         <v>0</v>
       </c>
@@ -1068,11 +1258,29 @@
       <c r="N10" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="O10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
@@ -1112,11 +1320,29 @@
       <c r="N11" t="s">
         <v>0</v>
       </c>
-      <c r="O11" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="O11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
@@ -1156,139 +1382,221 @@
       <c r="N12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="O12" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15"/>
-    <row r="14" spans="1:15"/>
-    <row r="15" spans="1:15"/>
-    <row r="16" spans="1:15"/>
-    <row r="17" spans="1:15"/>
-    <row r="18" spans="1:15">
+      <c r="O12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21"/>
+    <row r="14" spans="1:21"/>
+    <row r="15" spans="1:21"/>
+    <row r="16" spans="1:21"/>
+    <row r="17" spans="1:21"/>
+    <row r="18" spans="1:21">
       <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21"/>
+    <row r="20" spans="1:21">
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="B21" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21"/>
+    <row r="24" spans="1:21">
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="B25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="B26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="B27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="B28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="B29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="B30" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="B31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="B32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="B33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="B34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="B35" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="B36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="B37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="B38" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="B39" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:15"/>
-    <row r="20" spans="1:15">
-      <c r="B20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="B21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="C39" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="B40" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="B22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="C40" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="B41" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="B23" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="13" t="s">
+      <c r="C41" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="B42" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="B24" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="13" t="s">
+      <c r="C42" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="B43" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="B25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="13" t="s">
+      <c r="C43" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="B44" s="9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="B26" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="B27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="B28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="B29" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="B30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="B31" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="B32" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="B33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="B34" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>56</v>
+      <c r="C44" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1610,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1311,40 +1619,45 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="4"/>
-    <col customWidth="1" max="2" min="2" width="60"/>
-    <col customWidth="1" max="3" min="3" width="61"/>
-    <col customWidth="1" max="4" min="4" width="21"/>
-    <col customWidth="1" max="5" min="5" width="21"/>
-    <col customWidth="1" max="6" min="6" width="15"/>
-    <col customWidth="1" max="7" min="7" width="11"/>
-    <col customWidth="1" max="8" min="8" width="11"/>
-    <col customWidth="1" max="9" min="9" width="14"/>
-    <col customWidth="1" max="10" min="10" width="20"/>
-    <col customWidth="1" max="11" min="11" width="15"/>
-    <col customWidth="1" max="12" min="12" width="13"/>
+    <col customWidth="1" max="2" min="2" width="62"/>
+    <col customWidth="1" max="3" min="3" width="62"/>
+    <col customWidth="1" max="4" min="4" width="11"/>
+    <col customWidth="1" max="5" min="5" width="19"/>
+    <col customWidth="1" max="6" min="6" width="14"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="9"/>
+    <col customWidth="1" max="9" min="9" width="7"/>
+    <col customWidth="1" max="10" min="10" width="21"/>
+    <col customWidth="1" max="11" min="11" width="21"/>
+    <col customWidth="1" max="12" min="12" width="15"/>
+    <col customWidth="1" max="13" min="13" width="11"/>
+    <col customWidth="1" max="14" min="14" width="11"/>
+    <col customWidth="1" max="15" min="15" width="14"/>
+    <col customWidth="1" max="16" min="16" width="20"/>
+    <col customWidth="1" max="17" min="17" width="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12"/>
-    <row r="3" spans="1:12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17"/>
+    <row r="3" spans="1:17">
       <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="B4" s="1" t="n"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:17">
       <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12"/>
-    <row r="7" spans="1:12">
+    <row r="6" spans="1:17"/>
+    <row r="7" spans="1:17">
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1375,11 +1688,26 @@
       <c r="K7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="B8" s="6" t="s">
         <v>0</v>
       </c>
@@ -1410,11 +1738,26 @@
       <c r="K8" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="L8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="B9" s="6" t="s">
         <v>0</v>
       </c>
@@ -1445,11 +1788,26 @@
       <c r="K9" t="s">
         <v>0</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="L9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="B10" s="6" t="s">
         <v>0</v>
       </c>
@@ -1480,11 +1838,26 @@
       <c r="K10" t="s">
         <v>0</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="L10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
@@ -1515,11 +1888,26 @@
       <c r="K11" t="s">
         <v>0</v>
       </c>
-      <c r="L11" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="L11" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="B12" s="6" t="s">
         <v>0</v>
       </c>
@@ -1550,11 +1938,26 @@
       <c r="K12" t="s">
         <v>0</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="L12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1585,11 +1988,26 @@
       <c r="K13" t="s">
         <v>0</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="L13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
@@ -1620,11 +2038,26 @@
       <c r="K14" t="s">
         <v>0</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="L14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
@@ -1655,11 +2088,26 @@
       <c r="K15" t="s">
         <v>0</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="L15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="B16" s="6" t="s">
         <v>0</v>
       </c>
@@ -1690,11 +2138,26 @@
       <c r="K16" t="s">
         <v>0</v>
       </c>
-      <c r="L16" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="B17" s="6" t="s">
         <v>0</v>
       </c>
@@ -1725,11 +2188,26 @@
       <c r="K17" t="s">
         <v>0</v>
       </c>
-      <c r="L17" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="L17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="B18" s="6" t="s">
         <v>0</v>
       </c>
@@ -1760,11 +2238,26 @@
       <c r="K18" t="s">
         <v>0</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="L18" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
@@ -1795,11 +2288,26 @@
       <c r="K19" t="s">
         <v>0</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="L19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="B20" s="6" t="s">
         <v>0</v>
       </c>
@@ -1830,11 +2338,26 @@
       <c r="K20" t="s">
         <v>0</v>
       </c>
-      <c r="L20" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="L20" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="B21" s="6" t="s">
         <v>0</v>
       </c>
@@ -1865,11 +2388,26 @@
       <c r="K21" t="s">
         <v>0</v>
       </c>
-      <c r="L21" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="L21" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="B22" s="6" t="s">
         <v>0</v>
       </c>
@@ -1900,11 +2438,26 @@
       <c r="K22" t="s">
         <v>0</v>
       </c>
-      <c r="L22" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="L22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M22" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="B23" s="6" t="s">
         <v>0</v>
       </c>
@@ -1935,11 +2488,26 @@
       <c r="K23" t="s">
         <v>0</v>
       </c>
-      <c r="L23" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="L23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="B24" s="6" t="s">
         <v>0</v>
       </c>
@@ -1970,11 +2538,26 @@
       <c r="K24" t="s">
         <v>0</v>
       </c>
-      <c r="L24" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="L24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>0</v>
+      </c>
+      <c r="P24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="B25" s="6" t="s">
         <v>0</v>
       </c>
@@ -2005,11 +2588,26 @@
       <c r="K25" t="s">
         <v>0</v>
       </c>
-      <c r="L25" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="L25" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="B26" s="6" t="s">
         <v>0</v>
       </c>
@@ -2040,11 +2638,26 @@
       <c r="K26" t="s">
         <v>0</v>
       </c>
-      <c r="L26" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="L26" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -2075,11 +2688,26 @@
       <c r="K27" t="s">
         <v>0</v>
       </c>
-      <c r="L27" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="L27" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="B28" s="6" t="s">
         <v>0</v>
       </c>
@@ -2110,11 +2738,26 @@
       <c r="K28" t="s">
         <v>0</v>
       </c>
-      <c r="L28" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="L28" t="s">
+        <v>0</v>
+      </c>
+      <c r="M28" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="B29" s="6" t="s">
         <v>0</v>
       </c>
@@ -2145,11 +2788,26 @@
       <c r="K29" t="s">
         <v>0</v>
       </c>
-      <c r="L29" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="L29" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>0</v>
+      </c>
+      <c r="O29" t="s">
+        <v>0</v>
+      </c>
+      <c r="P29" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="B30" s="6" t="s">
         <v>0</v>
       </c>
@@ -2180,11 +2838,26 @@
       <c r="K30" t="s">
         <v>0</v>
       </c>
-      <c r="L30" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="L30" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>0</v>
+      </c>
+      <c r="O30" t="s">
+        <v>0</v>
+      </c>
+      <c r="P30" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="B31" s="6" t="s">
         <v>0</v>
       </c>
@@ -2215,11 +2888,26 @@
       <c r="K31" t="s">
         <v>0</v>
       </c>
-      <c r="L31" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="L31" t="s">
+        <v>0</v>
+      </c>
+      <c r="M31" t="s">
+        <v>0</v>
+      </c>
+      <c r="N31" t="s">
+        <v>0</v>
+      </c>
+      <c r="O31" t="s">
+        <v>0</v>
+      </c>
+      <c r="P31" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="B32" s="6" t="s">
         <v>0</v>
       </c>
@@ -2250,11 +2938,26 @@
       <c r="K32" t="s">
         <v>0</v>
       </c>
-      <c r="L32" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="L32" t="s">
+        <v>0</v>
+      </c>
+      <c r="M32" t="s">
+        <v>0</v>
+      </c>
+      <c r="N32" t="s">
+        <v>0</v>
+      </c>
+      <c r="O32" t="s">
+        <v>0</v>
+      </c>
+      <c r="P32" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="B33" s="6" t="s">
         <v>0</v>
       </c>
@@ -2285,11 +2988,26 @@
       <c r="K33" t="s">
         <v>0</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="L33" t="s">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" t="s">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>0</v>
+      </c>
+      <c r="P33" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="B34" s="6" t="s">
         <v>0</v>
       </c>
@@ -2320,11 +3038,26 @@
       <c r="K34" t="s">
         <v>0</v>
       </c>
-      <c r="L34" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="L34" t="s">
+        <v>0</v>
+      </c>
+      <c r="M34" t="s">
+        <v>0</v>
+      </c>
+      <c r="N34" t="s">
+        <v>0</v>
+      </c>
+      <c r="O34" t="s">
+        <v>0</v>
+      </c>
+      <c r="P34" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="B35" s="6" t="s">
         <v>0</v>
       </c>
@@ -2355,11 +3088,26 @@
       <c r="K35" t="s">
         <v>0</v>
       </c>
-      <c r="L35" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="L35" t="s">
+        <v>0</v>
+      </c>
+      <c r="M35" t="s">
+        <v>0</v>
+      </c>
+      <c r="N35" t="s">
+        <v>0</v>
+      </c>
+      <c r="O35" t="s">
+        <v>0</v>
+      </c>
+      <c r="P35" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="B36" s="6" t="s">
         <v>0</v>
       </c>
@@ -2390,11 +3138,26 @@
       <c r="K36" t="s">
         <v>0</v>
       </c>
-      <c r="L36" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="L36" t="s">
+        <v>0</v>
+      </c>
+      <c r="M36" t="s">
+        <v>0</v>
+      </c>
+      <c r="N36" t="s">
+        <v>0</v>
+      </c>
+      <c r="O36" t="s">
+        <v>0</v>
+      </c>
+      <c r="P36" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="B37" s="6" t="s">
         <v>0</v>
       </c>
@@ -2425,11 +3188,26 @@
       <c r="K37" t="s">
         <v>0</v>
       </c>
-      <c r="L37" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="L37" t="s">
+        <v>0</v>
+      </c>
+      <c r="M37" t="s">
+        <v>0</v>
+      </c>
+      <c r="N37" t="s">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
+        <v>0</v>
+      </c>
+      <c r="P37" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="B38" s="6" t="s">
         <v>0</v>
       </c>
@@ -2460,11 +3238,26 @@
       <c r="K38" t="s">
         <v>0</v>
       </c>
-      <c r="L38" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="L38" t="s">
+        <v>0</v>
+      </c>
+      <c r="M38" t="s">
+        <v>0</v>
+      </c>
+      <c r="N38" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" t="s">
+        <v>0</v>
+      </c>
+      <c r="P38" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="B39" s="6" t="s">
         <v>0</v>
       </c>
@@ -2495,11 +3288,26 @@
       <c r="K39" t="s">
         <v>0</v>
       </c>
-      <c r="L39" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="L39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O39" t="s">
+        <v>0</v>
+      </c>
+      <c r="P39" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="B40" s="6" t="s">
         <v>0</v>
       </c>
@@ -2530,11 +3338,26 @@
       <c r="K40" t="s">
         <v>0</v>
       </c>
-      <c r="L40" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="L40" t="s">
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>0</v>
+      </c>
+      <c r="N40" t="s">
+        <v>0</v>
+      </c>
+      <c r="O40" t="s">
+        <v>0</v>
+      </c>
+      <c r="P40" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
       <c r="B41" s="6" t="s">
         <v>0</v>
       </c>
@@ -2565,11 +3388,26 @@
       <c r="K41" t="s">
         <v>0</v>
       </c>
-      <c r="L41" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="L41" t="s">
+        <v>0</v>
+      </c>
+      <c r="M41" t="s">
+        <v>0</v>
+      </c>
+      <c r="N41" t="s">
+        <v>0</v>
+      </c>
+      <c r="O41" t="s">
+        <v>0</v>
+      </c>
+      <c r="P41" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
       <c r="B42" s="6" t="s">
         <v>0</v>
       </c>
@@ -2600,11 +3438,26 @@
       <c r="K42" t="s">
         <v>0</v>
       </c>
-      <c r="L42" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="L42" t="s">
+        <v>0</v>
+      </c>
+      <c r="M42" t="s">
+        <v>0</v>
+      </c>
+      <c r="N42" t="s">
+        <v>0</v>
+      </c>
+      <c r="O42" t="s">
+        <v>0</v>
+      </c>
+      <c r="P42" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
       <c r="B43" s="6" t="s">
         <v>0</v>
       </c>
@@ -2635,11 +3488,26 @@
       <c r="K43" t="s">
         <v>0</v>
       </c>
-      <c r="L43" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="L43" t="s">
+        <v>0</v>
+      </c>
+      <c r="M43" t="s">
+        <v>0</v>
+      </c>
+      <c r="N43" t="s">
+        <v>0</v>
+      </c>
+      <c r="O43" t="s">
+        <v>0</v>
+      </c>
+      <c r="P43" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="B44" s="6" t="s">
         <v>0</v>
       </c>
@@ -2670,11 +3538,26 @@
       <c r="K44" t="s">
         <v>0</v>
       </c>
-      <c r="L44" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="L44" t="s">
+        <v>0</v>
+      </c>
+      <c r="M44" t="s">
+        <v>0</v>
+      </c>
+      <c r="N44" t="s">
+        <v>0</v>
+      </c>
+      <c r="O44" t="s">
+        <v>0</v>
+      </c>
+      <c r="P44" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
       <c r="B45" s="6" t="s">
         <v>0</v>
       </c>
@@ -2705,11 +3588,26 @@
       <c r="K45" t="s">
         <v>0</v>
       </c>
-      <c r="L45" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="L45" t="s">
+        <v>0</v>
+      </c>
+      <c r="M45" t="s">
+        <v>0</v>
+      </c>
+      <c r="N45" t="s">
+        <v>0</v>
+      </c>
+      <c r="O45" t="s">
+        <v>0</v>
+      </c>
+      <c r="P45" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
       <c r="B46" s="6" t="s">
         <v>0</v>
       </c>
@@ -2740,11 +3638,26 @@
       <c r="K46" t="s">
         <v>0</v>
       </c>
-      <c r="L46" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="L46" t="s">
+        <v>0</v>
+      </c>
+      <c r="M46" t="s">
+        <v>0</v>
+      </c>
+      <c r="N46" t="s">
+        <v>0</v>
+      </c>
+      <c r="O46" t="s">
+        <v>0</v>
+      </c>
+      <c r="P46" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
       <c r="B47" s="6" t="s">
         <v>0</v>
       </c>
@@ -2775,11 +3688,26 @@
       <c r="K47" t="s">
         <v>0</v>
       </c>
-      <c r="L47" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="L47" t="s">
+        <v>0</v>
+      </c>
+      <c r="M47" t="s">
+        <v>0</v>
+      </c>
+      <c r="N47" t="s">
+        <v>0</v>
+      </c>
+      <c r="O47" t="s">
+        <v>0</v>
+      </c>
+      <c r="P47" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
       <c r="B48" s="6" t="s">
         <v>0</v>
       </c>
@@ -2810,11 +3738,26 @@
       <c r="K48" t="s">
         <v>0</v>
       </c>
-      <c r="L48" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="L48" t="s">
+        <v>0</v>
+      </c>
+      <c r="M48" t="s">
+        <v>0</v>
+      </c>
+      <c r="N48" t="s">
+        <v>0</v>
+      </c>
+      <c r="O48" t="s">
+        <v>0</v>
+      </c>
+      <c r="P48" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
       <c r="B49" s="6" t="s">
         <v>0</v>
       </c>
@@ -2845,11 +3788,26 @@
       <c r="K49" t="s">
         <v>0</v>
       </c>
-      <c r="L49" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="L49" t="s">
+        <v>0</v>
+      </c>
+      <c r="M49" t="s">
+        <v>0</v>
+      </c>
+      <c r="N49" t="s">
+        <v>0</v>
+      </c>
+      <c r="O49" t="s">
+        <v>0</v>
+      </c>
+      <c r="P49" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
       <c r="B50" s="6" t="s">
         <v>0</v>
       </c>
@@ -2880,11 +3838,26 @@
       <c r="K50" t="s">
         <v>0</v>
       </c>
-      <c r="L50" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="L50" t="s">
+        <v>0</v>
+      </c>
+      <c r="M50" t="s">
+        <v>0</v>
+      </c>
+      <c r="N50" t="s">
+        <v>0</v>
+      </c>
+      <c r="O50" t="s">
+        <v>0</v>
+      </c>
+      <c r="P50" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
       <c r="B51" s="6" t="s">
         <v>0</v>
       </c>
@@ -2915,11 +3888,26 @@
       <c r="K51" t="s">
         <v>0</v>
       </c>
-      <c r="L51" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="L51" t="s">
+        <v>0</v>
+      </c>
+      <c r="M51" t="s">
+        <v>0</v>
+      </c>
+      <c r="N51" t="s">
+        <v>0</v>
+      </c>
+      <c r="O51" t="s">
+        <v>0</v>
+      </c>
+      <c r="P51" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
       <c r="B52" s="6" t="s">
         <v>0</v>
       </c>
@@ -2950,11 +3938,26 @@
       <c r="K52" t="s">
         <v>0</v>
       </c>
-      <c r="L52" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="L52" t="s">
+        <v>0</v>
+      </c>
+      <c r="M52" t="s">
+        <v>0</v>
+      </c>
+      <c r="N52" t="s">
+        <v>0</v>
+      </c>
+      <c r="O52" t="s">
+        <v>0</v>
+      </c>
+      <c r="P52" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
       <c r="B53" s="6" t="s">
         <v>0</v>
       </c>
@@ -2985,11 +3988,26 @@
       <c r="K53" t="s">
         <v>0</v>
       </c>
-      <c r="L53" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="L53" t="s">
+        <v>0</v>
+      </c>
+      <c r="M53" t="s">
+        <v>0</v>
+      </c>
+      <c r="N53" t="s">
+        <v>0</v>
+      </c>
+      <c r="O53" t="s">
+        <v>0</v>
+      </c>
+      <c r="P53" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
       <c r="B54" s="6" t="s">
         <v>0</v>
       </c>
@@ -3020,11 +4038,26 @@
       <c r="K54" t="s">
         <v>0</v>
       </c>
-      <c r="L54" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="L54" t="s">
+        <v>0</v>
+      </c>
+      <c r="M54" t="s">
+        <v>0</v>
+      </c>
+      <c r="N54" t="s">
+        <v>0</v>
+      </c>
+      <c r="O54" t="s">
+        <v>0</v>
+      </c>
+      <c r="P54" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
       <c r="B55" s="6" t="s">
         <v>0</v>
       </c>
@@ -3055,11 +4088,26 @@
       <c r="K55" t="s">
         <v>0</v>
       </c>
-      <c r="L55" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="L55" t="s">
+        <v>0</v>
+      </c>
+      <c r="M55" t="s">
+        <v>0</v>
+      </c>
+      <c r="N55" t="s">
+        <v>0</v>
+      </c>
+      <c r="O55" t="s">
+        <v>0</v>
+      </c>
+      <c r="P55" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
       <c r="B56" s="6" t="s">
         <v>0</v>
       </c>
@@ -3090,11 +4138,26 @@
       <c r="K56" t="s">
         <v>0</v>
       </c>
-      <c r="L56" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="L56" t="s">
+        <v>0</v>
+      </c>
+      <c r="M56" t="s">
+        <v>0</v>
+      </c>
+      <c r="N56" t="s">
+        <v>0</v>
+      </c>
+      <c r="O56" t="s">
+        <v>0</v>
+      </c>
+      <c r="P56" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
       <c r="B57" s="9" t="s">
         <v>0</v>
       </c>
@@ -3125,115 +4188,188 @@
       <c r="K57" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="L57" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12"/>
-    <row r="59" spans="1:12"/>
-    <row r="60" spans="1:12"/>
-    <row r="61" spans="1:12"/>
-    <row r="62" spans="1:12"/>
-    <row r="63" spans="1:12">
+      <c r="L57" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O57" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P57" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17"/>
+    <row r="59" spans="1:17"/>
+    <row r="60" spans="1:17"/>
+    <row r="61" spans="1:17"/>
+    <row r="62" spans="1:17"/>
+    <row r="63" spans="1:17">
       <c r="B63" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12"/>
-    <row r="65" spans="1:12">
-      <c r="B65" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="B64" s="1" t="n"/>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="B65" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="B66" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="B67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17"/>
+    <row r="69" spans="1:17">
+      <c r="B69" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
-      <c r="B66" s="6" t="s">
+    <row r="70" spans="1:17">
+      <c r="B70" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C70" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="B71" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
+      <c r="B72" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="B73" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
+      <c r="B74" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="B75" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17">
+      <c r="B76" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17">
+      <c r="B77" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17">
+      <c r="B78" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
-      <c r="B67" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12">
-      <c r="B68" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
-      <c r="B69" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12">
-      <c r="B70" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12">
-      <c r="B71" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="B72" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12">
-      <c r="B73" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="B74" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C74" s="13" t="s">
+    <row r="79" spans="1:17">
+      <c r="B79" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
-      <c r="B75" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12">
-      <c r="B76" s="9" t="s">
+    <row r="80" spans="1:17">
+      <c r="B80" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C76" s="11" t="s">
-        <v>53</v>
+      <c r="C80" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17">
+      <c r="B81" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17">
+      <c r="B82" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
+      <c r="B83" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17">
+      <c r="B84" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17">
+      <c r="B85" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3247,7 +4383,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3256,9 +4392,77 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="2"/>
+    <col customWidth="1" max="2" min="2" width="57"/>
+    <col customWidth="1" max="3" min="3" width="61"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1"/>
+    <row r="1" spans="1:4"/>
+    <row r="2" spans="1:4"/>
+    <row r="3" spans="1:4">
+      <c r="B3" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4"/>
+    <row r="5" spans="1:4">
+      <c r="B5" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4"/>
+    <row r="7" spans="1:4">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4"/>
+    <row r="12" spans="1:4"/>
+    <row r="13" spans="1:4"/>
+    <row r="14" spans="1:4"/>
+    <row r="15" spans="1:4"/>
+    <row r="16" spans="1:4">
+      <c r="B16" s="1" t="n"/>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates for v1.2. Introduction of inference tool guidelines.
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -8,9 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Submission" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Inferences" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Genotype" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Tool Settings" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Repertoire" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Inferences" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Genotype" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Tool Settings" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -108,6 +109,93 @@
 submission, eg additional info requested, when reviewed, etc</t>
   </si>
   <si>
+    <t>Repertoire</t>
+  </si>
+  <si>
+    <t>Please provide details of the repertoire from which
+inferences were made, and the methods by which it was
+constructed.</t>
+  </si>
+  <si>
+    <t>pub_ids</t>
+  </si>
+  <si>
+    <t>PubMed ifs of peer-reviewed publications describing this
+dataset</t>
+  </si>
+  <si>
+    <t>repository_name</t>
+  </si>
+  <si>
+    <t>Name of the repository holding the sequence dataset</t>
+  </si>
+  <si>
+    <t>repository_id</t>
+  </si>
+  <si>
+    <t>Id or serial number of the sequence dataset within the
+repository</t>
+  </si>
+  <si>
+    <t>dataset_url</t>
+  </si>
+  <si>
+    <t>URL of the sequence dataset (if any)</t>
+  </si>
+  <si>
+    <t>dataset_doi</t>
+  </si>
+  <si>
+    <t>doi of the sequence dataset (if any)</t>
+  </si>
+  <si>
+    <t>miarr_compliant</t>
+  </si>
+  <si>
+    <t>TRUE if the repertoire dataset and associated metadata is in
+miairr format</t>
+  </si>
+  <si>
+    <t>sequencing_platform</t>
+  </si>
+  <si>
+    <t>Designation of sequencing instrument used</t>
+  </si>
+  <si>
+    <t>read_length</t>
+  </si>
+  <si>
+    <t>Read length in bases for each direction</t>
+  </si>
+  <si>
+    <t>forward_primer_set</t>
+  </si>
+  <si>
+    <t>sequences of forward pcr primers used for sequence
+amplification</t>
+  </si>
+  <si>
+    <t>reverse_primer_set</t>
+  </si>
+  <si>
+    <t>sequences of reverse pcr primers used for sequence
+amplification</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Notes relating to the dataset, for example covering details
+of origin or processing methods not described in
+publications or sequence depositions</t>
+  </si>
+  <si>
+    <t>IARC_repertoire_id</t>
+  </si>
+  <si>
+    <t>Unique ID of the repertoire dataset, allocated by IARC</t>
+  </si>
+  <si>
     <t>Inferred Sequences</t>
   </si>
   <si>
@@ -115,12 +203,25 @@
 the meaning and format of each field</t>
   </si>
   <si>
+    <t>The table should be used to describe sequences inferred from
+a single invididual, in a single genotype. If inferences are
+made from multiple individuals and/or multiple genotypes,</t>
+  </si>
+  <si>
+    <t>please create a separate table on this tab for each
+genotyope from which inferences are made, and cross-
+reference to separate genotype tables on the genotype tab.</t>
+  </si>
+  <si>
+    <t>Subject id:</t>
+  </si>
+  <si>
+    <t>Genotype id (as listed on the Genotype tab):</t>
+  </si>
+  <si>
     <t>sequence_id</t>
   </si>
   <si>
-    <t>subject_id</t>
-  </si>
-  <si>
     <t>sequences</t>
   </si>
   <si>
@@ -167,12 +268,6 @@
   </si>
   <si>
     <t>phred_score</t>
-  </si>
-  <si>
-    <t>repository_name</t>
-  </si>
-  <si>
-    <t>repository_id</t>
   </si>
   <si>
     <t>deposited_version</t>
@@ -198,12 +293,6 @@
 follow any particular format)</t>
   </si>
   <si>
-    <t>Identifier of the subject from which this sequence was
-inferred (if inferred from more than one subject, please
-complete separate Inferred_Sequence records for each
-subject)</t>
-  </si>
-  <si>
     <t>Overall number of sequences assigned to this allele</t>
   </si>
   <si>
@@ -280,6 +369,21 @@
   </si>
   <si>
     <t>Genotype</t>
+  </si>
+  <si>
+    <t>If inferences are made from multiple genotypes, please
+create separate tables for each genotype, and cross-
+reference to the inferences made from each one on the
+Inferences tab.</t>
+  </si>
+  <si>
+    <t>Genotype Id:</t>
+  </si>
+  <si>
+    <t>Subject Id (as listed on Inferences tab):</t>
+  </si>
+  <si>
+    <t>subject_id</t>
   </si>
   <si>
     <t>Notes on FIelds</t>
@@ -824,7 +928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -857,50 +961,40 @@
       </c>
     </row>
     <row r="6" spans="1:4"/>
-    <row r="7" spans="1:4">
-      <c r="B7" t="s">
+    <row r="7" spans="1:4"/>
+    <row r="8" spans="1:4">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C8" s="2" t="n">
         <v>1.1</v>
       </c>
     </row>
-    <row r="8" spans="1:4"/>
     <row r="9" spans="1:4"/>
-    <row r="10" spans="1:4">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:4"/>
+    <row r="11" spans="1:4">
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4"/>
-    <row r="12" spans="1:4">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="1:4"/>
+    <row r="13" spans="1:4">
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>0</v>
@@ -908,10 +1002,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>0</v>
@@ -919,10 +1013,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>0</v>
@@ -930,10 +1024,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="B17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>0</v>
@@ -941,10 +1035,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="B18" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>0</v>
@@ -952,10 +1046,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="B19" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>0</v>
@@ -963,10 +1057,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="B20" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>0</v>
@@ -974,27 +1068,38 @@
     </row>
     <row r="21" spans="1:4">
       <c r="B21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="B22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="B22" s="9" t="s">
+      <c r="D22" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4"/>
+      <c r="D23" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1006,7 +1111,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W46"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1014,667 +1119,170 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="3"/>
-    <col customWidth="1" max="2" min="2" width="62"/>
+    <col customWidth="1" max="1" min="1" width="2"/>
+    <col customWidth="1" max="2" min="2" width="55"/>
     <col customWidth="1" max="3" min="3" width="62"/>
-    <col customWidth="1" max="4" min="4" width="11"/>
-    <col customWidth="1" max="5" min="5" width="19"/>
-    <col customWidth="1" max="6" min="6" width="14"/>
-    <col customWidth="1" max="7" min="7" width="9"/>
-    <col customWidth="1" max="8" min="8" width="9"/>
-    <col customWidth="1" max="9" min="9" width="7"/>
-    <col customWidth="1" max="10" min="10" width="21"/>
-    <col customWidth="1" max="11" min="11" width="21"/>
-    <col customWidth="1" max="12" min="12" width="20"/>
-    <col customWidth="1" max="13" min="13" width="11"/>
-    <col customWidth="1" max="14" min="14" width="11"/>
-    <col customWidth="1" max="15" min="15" width="14"/>
-    <col customWidth="1" max="16" min="16" width="19"/>
-    <col customWidth="1" max="17" min="17" width="19"/>
-    <col customWidth="1" max="18" min="18" width="13"/>
-    <col customWidth="1" max="19" min="19" width="13"/>
-    <col customWidth="1" max="20" min="20" width="17"/>
-    <col customWidth="1" max="21" min="21" width="15"/>
-    <col customWidth="1" max="22" min="22" width="19"/>
-    <col customWidth="1" max="23" min="23" width="15"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23"/>
-    <row r="2" spans="1:23"/>
-    <row r="3" spans="1:23">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:4"/>
+    <row r="2" spans="1:4"/>
+    <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:4">
       <c r="B4" s="1" t="n"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:4">
       <c r="B5" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:23"/>
-    <row r="7" spans="1:23">
-      <c r="B7" s="3" t="s">
+    <row r="6" spans="1:4"/>
+    <row r="7" spans="1:4"/>
+    <row r="8" spans="1:4">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D9" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="D10" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="C11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="D11" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="D12" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="D13" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="C14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="D14" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="D15" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="D16" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="C17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="D17" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="B18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="U7" s="4" t="s">
+      <c r="C18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="V7" s="4" t="s">
+      <c r="D18" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="B19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W7" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="B8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
-        <v>0</v>
-      </c>
-      <c r="O8" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" t="s">
-        <v>0</v>
-      </c>
-      <c r="S8" t="s">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>0</v>
-      </c>
-      <c r="U8" t="s">
-        <v>0</v>
-      </c>
-      <c r="V8" t="s">
-        <v>0</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="B9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>0</v>
-      </c>
-      <c r="S9" t="s">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
-        <v>0</v>
-      </c>
-      <c r="U9" t="s">
-        <v>0</v>
-      </c>
-      <c r="V9" t="s">
-        <v>0</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="B10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>0</v>
-      </c>
-      <c r="R10" t="s">
-        <v>0</v>
-      </c>
-      <c r="S10" t="s">
-        <v>0</v>
-      </c>
-      <c r="T10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U10" t="s">
-        <v>0</v>
-      </c>
-      <c r="V10" t="s">
-        <v>0</v>
-      </c>
-      <c r="W10" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="B11" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" t="s">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>0</v>
-      </c>
-      <c r="S11" t="s">
-        <v>0</v>
-      </c>
-      <c r="T11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V11" t="s">
-        <v>0</v>
-      </c>
-      <c r="W11" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="B12" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="S12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="T12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="U12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="W12" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23"/>
-    <row r="14" spans="1:23"/>
-    <row r="15" spans="1:23"/>
-    <row r="16" spans="1:23"/>
-    <row r="17" spans="1:23"/>
-    <row r="18" spans="1:23">
-      <c r="B18" s="1" t="s">
+      <c r="C19" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:23"/>
-    <row r="20" spans="1:23">
-      <c r="B20" t="s">
+      <c r="D19" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" s="9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:23">
-      <c r="B21" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:23">
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23"/>
-    <row r="24" spans="1:23">
-      <c r="B24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23">
-      <c r="B25" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23">
-      <c r="B26" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23">
-      <c r="B27" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23">
-      <c r="B28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23">
-      <c r="B29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23">
-      <c r="B30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23">
-      <c r="B31" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23">
-      <c r="B32" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23">
-      <c r="B33" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23">
-      <c r="B34" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23">
-      <c r="B35" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23">
-      <c r="B36" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23">
-      <c r="B37" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23">
-      <c r="B38" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23">
-      <c r="B39" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23">
-      <c r="B40" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23">
-      <c r="B41" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23">
-      <c r="B42" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23">
-      <c r="B43" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23">
-      <c r="B44" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23">
-      <c r="B45" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23">
-      <c r="B46" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>27</v>
+      <c r="D20" s="11" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1688,7 +1296,682 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:V49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="3"/>
+    <col customWidth="1" max="2" min="2" width="62"/>
+    <col customWidth="1" max="3" min="3" width="62"/>
+    <col customWidth="1" max="4" min="4" width="19"/>
+    <col customWidth="1" max="5" min="5" width="14"/>
+    <col customWidth="1" max="6" min="6" width="9"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="7"/>
+    <col customWidth="1" max="9" min="9" width="21"/>
+    <col customWidth="1" max="10" min="10" width="21"/>
+    <col customWidth="1" max="11" min="11" width="20"/>
+    <col customWidth="1" max="12" min="12" width="11"/>
+    <col customWidth="1" max="13" min="13" width="11"/>
+    <col customWidth="1" max="14" min="14" width="14"/>
+    <col customWidth="1" max="15" min="15" width="19"/>
+    <col customWidth="1" max="16" min="16" width="19"/>
+    <col customWidth="1" max="17" min="17" width="13"/>
+    <col customWidth="1" max="18" min="18" width="13"/>
+    <col customWidth="1" max="19" min="19" width="17"/>
+    <col customWidth="1" max="20" min="20" width="15"/>
+    <col customWidth="1" max="21" min="21" width="19"/>
+    <col customWidth="1" max="22" min="22" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22"/>
+    <row r="2" spans="1:22"/>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="B4" s="1" t="n"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="B5" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="B6" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="B7" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22"/>
+    <row r="9" spans="1:22">
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="B11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="B12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
+        <v>0</v>
+      </c>
+      <c r="V12" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="B13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>0</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="B14" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>0</v>
+      </c>
+      <c r="V14" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="B15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="B16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="V16" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22"/>
+    <row r="18" spans="1:22"/>
+    <row r="19" spans="1:22"/>
+    <row r="20" spans="1:22"/>
+    <row r="21" spans="1:22"/>
+    <row r="22" spans="1:22">
+      <c r="B22" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22"/>
+    <row r="24" spans="1:22">
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="B25" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22"/>
+    <row r="28" spans="1:22">
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="B29" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="B30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="B31" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="B32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="B33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
+      <c r="B34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="B35" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="B36" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="B37" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="B38" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
+      <c r="B39" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="B40" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="B41" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="B42" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="B43" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="B44" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="B45" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="B46" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="B47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="B48" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
+      <c r="B49" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1718,13 +2001,13 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:18"/>
     <row r="3" spans="1:18">
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1732,220 +2015,76 @@
     </row>
     <row r="5" spans="1:18">
       <c r="B5" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18"/>
-    <row r="7" spans="1:18">
-      <c r="B7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="B6" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18"/>
     <row r="8" spans="1:18">
-      <c r="B8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
-        <v>0</v>
-      </c>
-      <c r="O8" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>0</v>
+      <c r="B8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>0</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>0</v>
+      <c r="B9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="B10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>0</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>0</v>
+      <c r="B10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -4387,229 +4526,388 @@
       </c>
     </row>
     <row r="57" spans="1:18">
-      <c r="B57" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R57" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18"/>
-    <row r="59" spans="1:18"/>
-    <row r="60" spans="1:18"/>
+      <c r="B57" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>0</v>
+      </c>
+      <c r="G57" t="s">
+        <v>0</v>
+      </c>
+      <c r="H57" t="s">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>0</v>
+      </c>
+      <c r="K57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L57" t="s">
+        <v>0</v>
+      </c>
+      <c r="M57" t="s">
+        <v>0</v>
+      </c>
+      <c r="N57" t="s">
+        <v>0</v>
+      </c>
+      <c r="O57" t="s">
+        <v>0</v>
+      </c>
+      <c r="P57" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>0</v>
+      </c>
+      <c r="R57" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="B58" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>0</v>
+      </c>
+      <c r="G58" t="s">
+        <v>0</v>
+      </c>
+      <c r="H58" t="s">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>0</v>
+      </c>
+      <c r="K58" t="s">
+        <v>0</v>
+      </c>
+      <c r="L58" t="s">
+        <v>0</v>
+      </c>
+      <c r="M58" t="s">
+        <v>0</v>
+      </c>
+      <c r="N58" t="s">
+        <v>0</v>
+      </c>
+      <c r="O58" t="s">
+        <v>0</v>
+      </c>
+      <c r="P58" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>0</v>
+      </c>
+      <c r="R58" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="B59" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>0</v>
+      </c>
+      <c r="G59" t="s">
+        <v>0</v>
+      </c>
+      <c r="H59" t="s">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>0</v>
+      </c>
+      <c r="K59" t="s">
+        <v>0</v>
+      </c>
+      <c r="L59" t="s">
+        <v>0</v>
+      </c>
+      <c r="M59" t="s">
+        <v>0</v>
+      </c>
+      <c r="N59" t="s">
+        <v>0</v>
+      </c>
+      <c r="O59" t="s">
+        <v>0</v>
+      </c>
+      <c r="P59" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>0</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="B60" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R60" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="61" spans="1:18"/>
     <row r="62" spans="1:18"/>
-    <row r="63" spans="1:18">
-      <c r="B63" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18">
-      <c r="B64" s="1" t="n"/>
-    </row>
-    <row r="65" spans="1:18">
-      <c r="B65" t="s">
-        <v>79</v>
-      </c>
-    </row>
+    <row r="63" spans="1:18"/>
+    <row r="64" spans="1:18"/>
+    <row r="65" spans="1:18"/>
     <row r="66" spans="1:18">
-      <c r="B66" s="13" t="s">
-        <v>80</v>
+      <c r="B66" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:18">
-      <c r="B67" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18"/>
+      <c r="B67" s="1" t="n"/>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="B68" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="69" spans="1:18">
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
+      <c r="B70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18"/>
+    <row r="72" spans="1:18">
+      <c r="B72" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18">
-      <c r="B70" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18">
-      <c r="B71" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18">
-      <c r="B72" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:18">
       <c r="B73" s="6" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="B74" s="6" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:18">
       <c r="B75" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>85</v>
+        <v>61</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="B76" s="6" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:18">
       <c r="B77" s="6" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:18">
       <c r="B78" s="6" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:18">
       <c r="B79" s="6" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:18">
       <c r="B80" s="6" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:18">
       <c r="B81" s="6" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:18">
       <c r="B82" s="6" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:18">
       <c r="B83" s="6" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:18">
       <c r="B84" s="6" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:18">
       <c r="B85" s="6" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:18">
-      <c r="B86" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>71</v>
+      <c r="B86" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="B87" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="B88" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
+      <c r="B89" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -4617,7 +4915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4641,13 +4939,13 @@
     <row r="2" spans="1:4"/>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4"/>
     <row r="5" spans="1:4">
       <c r="B5" s="8" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:4"/>
@@ -4664,10 +4962,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="6" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>0</v>
@@ -4675,10 +4973,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="6" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>0</v>
@@ -4686,10 +4984,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="9" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Draft changes for v1.3
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -156,6 +156,12 @@
 miairr format</t>
   </si>
   <si>
+    <t>miairr_link</t>
+  </si>
+  <si>
+    <t>Link to miairr metadata, if available</t>
+  </si>
+  <si>
     <t>sequencing_platform</t>
   </si>
   <si>
@@ -187,7 +193,9 @@
   <si>
     <t>Notes relating to the dataset, for example covering details
 of origin or processing methods not described in
-publications or sequence depositions</t>
+publications or sequence depositions. Please provide details
+of cell types sequenced, or indicate clearly where this and
+related biosample information can be found.</t>
   </si>
   <si>
     <t>IARC_repertoire_id</t>
@@ -234,10 +242,13 @@
     <t>nt_diff</t>
   </si>
   <si>
+    <t>nt_substitutions</t>
+  </si>
+  <si>
     <t>aa_diff</t>
   </si>
   <si>
-    <t>cigar</t>
+    <t>aa_substitutions</t>
   </si>
   <si>
     <t>unmutated_frequency</t>
@@ -296,24 +307,28 @@
     <t>Overall number of sequences assigned to this allele</t>
   </si>
   <si>
-    <t>The closest reference gene and allele, based on percent
-identity</t>
+    <t>The closest reference gene and allele, as inferred by the
+tool</t>
   </si>
   <si>
     <t>The closest reference gene and allele that is in the
-subject's inferred genotype, based on percent identity</t>
+subject's inferred genotype, as inferred by the tool</t>
   </si>
   <si>
     <t>Number of nucleotides that differ between this sequence and
 the closest reference gene and allele</t>
   </si>
   <si>
+    <t>List of nucleotide substitutions (e.g. G112A) between this
+sequence and the closest reference gene and allele</t>
+  </si>
+  <si>
     <t>Number of amino acids that differ between this sequence and
 the closest reference gene and allele</t>
   </si>
   <si>
-    <t>Alignment between this sequence and the closest reference
-gene and allele (CIGAR string)</t>
+    <t>List of amino acid substitutions (e.g. A96N) between this
+sequence and the closest reference gene and allele</t>
   </si>
   <si>
     <t>The proportion of records in the sequence dataset matching
@@ -386,6 +401,9 @@
     <t>subject_id</t>
   </si>
   <si>
+    <t>cigar</t>
+  </si>
+  <si>
     <t>Notes on FIelds</t>
   </si>
   <si>
@@ -447,6 +465,14 @@
   </si>
   <si>
     <t>Version of the inference tool</t>
+  </si>
+  <si>
+    <t>starting_database</t>
+  </si>
+  <si>
+    <t>Starting germline database used by the tool (please specify
+where and when it was obtained, name, and version id, if
+any)</t>
   </si>
   <si>
     <t>tool_settings</t>
@@ -1111,7 +1137,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1245,7 +1271,7 @@
       <c r="B17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -1275,13 +1301,24 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1296,7 +1333,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1310,129 +1347,133 @@
     <col customWidth="1" max="4" min="4" width="19"/>
     <col customWidth="1" max="5" min="5" width="14"/>
     <col customWidth="1" max="6" min="6" width="9"/>
-    <col customWidth="1" max="7" min="7" width="9"/>
-    <col customWidth="1" max="8" min="8" width="7"/>
-    <col customWidth="1" max="9" min="9" width="21"/>
+    <col customWidth="1" max="7" min="7" width="18"/>
+    <col customWidth="1" max="8" min="8" width="9"/>
+    <col customWidth="1" max="9" min="9" width="18"/>
     <col customWidth="1" max="10" min="10" width="21"/>
-    <col customWidth="1" max="11" min="11" width="20"/>
-    <col customWidth="1" max="12" min="12" width="11"/>
+    <col customWidth="1" max="11" min="11" width="21"/>
+    <col customWidth="1" max="12" min="12" width="20"/>
     <col customWidth="1" max="13" min="13" width="11"/>
-    <col customWidth="1" max="14" min="14" width="14"/>
-    <col customWidth="1" max="15" min="15" width="19"/>
+    <col customWidth="1" max="14" min="14" width="11"/>
+    <col customWidth="1" max="15" min="15" width="14"/>
     <col customWidth="1" max="16" min="16" width="19"/>
-    <col customWidth="1" max="17" min="17" width="13"/>
+    <col customWidth="1" max="17" min="17" width="19"/>
     <col customWidth="1" max="18" min="18" width="13"/>
-    <col customWidth="1" max="19" min="19" width="17"/>
-    <col customWidth="1" max="20" min="20" width="15"/>
-    <col customWidth="1" max="21" min="21" width="19"/>
-    <col customWidth="1" max="22" min="22" width="15"/>
+    <col customWidth="1" max="19" min="19" width="13"/>
+    <col customWidth="1" max="20" min="20" width="17"/>
+    <col customWidth="1" max="21" min="21" width="15"/>
+    <col customWidth="1" max="22" min="22" width="19"/>
+    <col customWidth="1" max="23" min="23" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22"/>
-    <row r="2" spans="1:22"/>
-    <row r="3" spans="1:22">
+    <row r="1" spans="1:23"/>
+    <row r="2" spans="1:23"/>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="B4" s="1" t="n"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23">
       <c r="B5" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="B6" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="B7" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22"/>
-    <row r="9" spans="1:22">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23"/>
+    <row r="9" spans="1:23">
       <c r="B9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="B10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="S11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="U11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="U11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="V11" s="5" t="s">
+      <c r="V11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="W11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:23">
       <c r="B12" s="6" t="s">
         <v>0</v>
       </c>
@@ -1493,11 +1534,14 @@
       <c r="U12" t="s">
         <v>0</v>
       </c>
-      <c r="V12" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="V12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1558,11 +1602,14 @@
       <c r="U13" t="s">
         <v>0</v>
       </c>
-      <c r="V13" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="V13" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
@@ -1623,11 +1670,14 @@
       <c r="U14" t="s">
         <v>0</v>
       </c>
-      <c r="V14" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="V14" t="s">
+        <v>0</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
@@ -1688,11 +1738,14 @@
       <c r="U15" t="s">
         <v>0</v>
       </c>
-      <c r="V15" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="V15" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="B16" s="9" t="s">
         <v>0</v>
       </c>
@@ -1753,38 +1806,41 @@
       <c r="U16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="V16" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22"/>
-    <row r="18" spans="1:22"/>
-    <row r="19" spans="1:22"/>
-    <row r="20" spans="1:22"/>
-    <row r="21" spans="1:22"/>
-    <row r="22" spans="1:22">
+      <c r="V16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23"/>
+    <row r="18" spans="1:23"/>
+    <row r="19" spans="1:23"/>
+    <row r="20" spans="1:23"/>
+    <row r="21" spans="1:23"/>
+    <row r="22" spans="1:23">
       <c r="B22" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22"/>
-    <row r="24" spans="1:22">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23"/>
+    <row r="24" spans="1:23">
       <c r="B24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="B25" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="B26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22"/>
-    <row r="28" spans="1:22">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23"/>
+    <row r="28" spans="1:23">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
@@ -1792,171 +1848,179 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:23">
       <c r="B29" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="B30" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
       <c r="B31" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
       <c r="B32" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
       <c r="B33" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
       <c r="B34" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
       <c r="B35" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
       <c r="B36" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
       <c r="B37" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
       <c r="B38" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
       <c r="B39" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
       <c r="B40" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
       <c r="B41" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
       <c r="B42" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
       <c r="B43" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
       <c r="B44" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
+        <v>77</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
       <c r="B45" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22">
+        <v>78</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
       <c r="B46" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23">
+      <c r="B47" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C46" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22">
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23">
+      <c r="B48" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22">
-      <c r="B48" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="C48" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22">
-      <c r="B49" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23">
+      <c r="B49" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23">
+      <c r="B50" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C50" s="15" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2001,13 +2065,13 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:18"/>
     <row r="3" spans="1:18">
       <c r="B3" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -2015,76 +2079,76 @@
     </row>
     <row r="5" spans="1:18">
       <c r="B5" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:18"/>
     <row r="8" spans="1:18">
       <c r="B8" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="B9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -4744,7 +4808,7 @@
     <row r="65" spans="1:18"/>
     <row r="66" spans="1:18">
       <c r="B66" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:18">
@@ -4752,17 +4816,17 @@
     </row>
     <row r="68" spans="1:18">
       <c r="B68" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:18">
       <c r="B69" s="13" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="B70" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:18"/>
@@ -4776,138 +4840,138 @@
     </row>
     <row r="73" spans="1:18">
       <c r="B73" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="B74" s="6" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="1:18">
       <c r="B75" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="B76" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:18">
       <c r="B77" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:18">
       <c r="B78" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:18">
       <c r="B79" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="1:18">
       <c r="B80" s="6" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:18">
       <c r="B81" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:18">
       <c r="B82" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:18">
       <c r="B83" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:18">
       <c r="B84" s="6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:18">
       <c r="B85" s="6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="1:18">
       <c r="B86" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:18">
       <c r="B87" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:18">
       <c r="B88" s="6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:18">
       <c r="B89" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4921,7 +4985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4939,13 +5003,13 @@
     <row r="2" spans="1:4"/>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:4"/>
     <row r="5" spans="1:4">
       <c r="B5" s="8" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4"/>
@@ -4962,10 +5026,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>0</v>
@@ -4973,33 +5037,44 @@
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="6" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4"/>
+      <c r="B10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="12" spans="1:4"/>
     <row r="13" spans="1:4"/>
     <row r="14" spans="1:4"/>
     <row r="15" spans="1:4"/>
-    <row r="16" spans="1:4">
-      <c r="B16" s="1" t="n"/>
+    <row r="16" spans="1:4"/>
+    <row r="17" spans="1:4">
+      <c r="B17" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Add inferred sequence documentation
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="141">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -107,6 +107,34 @@
   <si>
     <t>Notes from IARC tracking overall progress of this
 submission, eg additional info requested, when reviewed, etc</t>
+  </si>
+  <si>
+    <t>Acknowledgements</t>
+  </si>
+  <si>
+    <t>Please list the individuals whose contribution to this work
+should be acknowledged</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>institution_name</t>
+  </si>
+  <si>
+    <t>ORCID_id</t>
+  </si>
+  <si>
+    <t>Explanation of fields</t>
+  </si>
+  <si>
+    <t>Full name of individual</t>
+  </si>
+  <si>
+    <t>Individual's department and institution name</t>
+  </si>
+  <si>
+    <t>Individual's ORCID Id, if available</t>
   </si>
   <si>
     <t>Repertoire</t>
@@ -293,10 +321,6 @@
     <t>'Number of sequences': where sequences are counted the count
 should be conducted after quality control  UMI processing
 and replicate/error cloud removal.</t>
-  </si>
-  <si>
-    <t>Question for review - should this be the number of distinct
-sequences or a molecule count?</t>
   </si>
   <si>
     <t>'Reference genes and alleles' - this is the set of genes and
@@ -954,7 +978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -963,7 +987,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="3"/>
-    <col customWidth="1" max="2" min="2" width="39"/>
+    <col customWidth="1" max="2" min="2" width="61"/>
     <col customWidth="1" max="3" min="3" width="62"/>
     <col customWidth="1" max="4" min="4" width="10"/>
   </cols>
@@ -993,7 +1017,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:4"/>
@@ -1126,6 +1150,180 @@
       </c>
     </row>
     <row r="24" spans="1:4"/>
+    <row r="25" spans="1:4"/>
+    <row r="26" spans="1:4"/>
+    <row r="27" spans="1:4">
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4"/>
+    <row r="30" spans="1:4">
+      <c r="B30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="B31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="B32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="B33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="B35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="B36" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="B39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="B40" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4"/>
+    <row r="42" spans="1:4"/>
+    <row r="43" spans="1:4">
+      <c r="B43" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="B45" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="B46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1155,7 +1353,7 @@
     <row r="2" spans="1:4"/>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1163,7 +1361,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="8" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4"/>
@@ -1181,10 +1379,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>0</v>
@@ -1192,10 +1390,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>0</v>
@@ -1203,10 +1401,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>0</v>
@@ -1214,10 +1412,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>0</v>
@@ -1225,10 +1423,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>0</v>
@@ -1236,10 +1434,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="B14" s="6" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>0</v>
@@ -1247,10 +1445,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="6" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>0</v>
@@ -1258,10 +1456,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="B16" s="6" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>0</v>
@@ -1269,10 +1467,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="B17" s="6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>0</v>
@@ -1280,10 +1478,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="B18" s="6" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>0</v>
@@ -1291,10 +1489,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="B19" s="6" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>0</v>
@@ -1302,10 +1500,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="B20" s="6" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>0</v>
@@ -1313,10 +1511,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="B21" s="9" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>0</v>
@@ -1333,7 +1531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X51"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1374,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -1382,96 +1580,96 @@
     </row>
     <row r="5" spans="1:24">
       <c r="B5" s="8" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="B6" s="8" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:24">
       <c r="B7" s="8" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:24"/>
     <row r="9" spans="1:24">
       <c r="B9" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:24">
       <c r="B10" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:24">
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="X11" s="5" t="s">
         <v>26</v>
@@ -1839,215 +2037,210 @@
     <row r="21" spans="1:24"/>
     <row r="22" spans="1:24">
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:24"/>
     <row r="24" spans="1:24">
       <c r="B24" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="B25" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24">
-      <c r="B26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24"/>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24"/>
+    <row r="27" spans="1:24">
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="28" spans="1:24">
-      <c r="B28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>6</v>
+      <c r="B28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:24">
       <c r="B29" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>86</v>
+        <v>72</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:24">
       <c r="B30" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:24">
       <c r="B31" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:24">
       <c r="B32" s="6" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:24">
       <c r="B33" s="6" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:24">
       <c r="B34" s="6" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:24">
       <c r="B35" s="6" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:24">
       <c r="B36" s="6" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:24">
       <c r="B37" s="6" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:24">
       <c r="B38" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="B39" s="6" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:24">
       <c r="B40" s="6" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:24">
       <c r="B41" s="6" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:24">
       <c r="B42" s="6" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:24">
       <c r="B43" s="6" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:24">
       <c r="B44" s="6" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:24">
       <c r="B45" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>102</v>
+        <v>88</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:24">
       <c r="B46" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>103</v>
+        <v>89</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:24">
       <c r="B47" s="6" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:24">
       <c r="B48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>105</v>
+        <v>43</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:24">
       <c r="B49" s="6" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:24">
-      <c r="B50" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24">
-      <c r="B51" s="9" t="s">
+      <c r="B50" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C50" s="15" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2094,13 +2287,13 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:20"/>
     <row r="3" spans="1:20">
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2108,82 +2301,82 @@
     </row>
     <row r="5" spans="1:20">
       <c r="B5" s="8" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="B6" s="8" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:20"/>
     <row r="8" spans="1:20">
       <c r="B8" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="B9" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -5143,7 +5336,7 @@
     <row r="65" spans="1:20"/>
     <row r="66" spans="1:20">
       <c r="B66" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:20">
@@ -5151,17 +5344,17 @@
     </row>
     <row r="68" spans="1:20">
       <c r="B68" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:20">
       <c r="B69" s="13" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:20">
       <c r="B70" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:20"/>
@@ -5175,154 +5368,154 @@
     </row>
     <row r="73" spans="1:20">
       <c r="B73" s="6" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:20">
       <c r="B74" s="6" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:20">
       <c r="B75" s="6" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:20">
       <c r="B76" s="6" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:20">
       <c r="B77" s="6" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:20">
       <c r="B78" s="6" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:20">
       <c r="B79" s="6" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:20">
       <c r="B80" s="6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:20">
       <c r="B81" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:20">
       <c r="B82" s="6" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:20">
       <c r="B83" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:20">
       <c r="B84" s="6" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:20">
       <c r="B85" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:20">
       <c r="B86" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:20">
       <c r="B87" s="6" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:20">
       <c r="B88" s="6" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:20">
       <c r="B89" s="6" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:20">
       <c r="B90" s="6" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:20">
       <c r="B91" s="9" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -5354,13 +5547,13 @@
     <row r="2" spans="1:4"/>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4"/>
     <row r="5" spans="1:4">
       <c r="B5" s="8" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4"/>
@@ -5377,10 +5570,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="6" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>0</v>
@@ -5388,10 +5581,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="6" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>0</v>
@@ -5399,10 +5592,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="6" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>0</v>
@@ -5410,10 +5603,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="9" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Updates fommowing IARC meeting on 2/6/2018 Remove IARC Repertoire Id Allow output from multiple tools in submission Add Notes page Small changes to field descriptions
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Inferences" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Genotype" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Tool Settings" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Notes" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="152">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -28,6 +29,10 @@
   </si>
   <si>
     <t>Please complete details on all tabs.</t>
+  </si>
+  <si>
+    <t>Please check the Notes tab for general guidance on
+completing this submission.</t>
   </si>
   <si>
     <t>Schema Version</t>
@@ -226,12 +231,6 @@
 related biosample information can be found.</t>
   </si>
   <si>
-    <t>IARC_repertoire_id</t>
-  </si>
-  <si>
-    <t>Unique ID of the repertoire dataset, allocated by IARC</t>
-  </si>
-  <si>
     <t>Inferred Sequences</t>
   </si>
   <si>
@@ -241,18 +240,17 @@
   <si>
     <t>The table should be used to describe sequences inferred from
 a single invididual, in a single genotype. If inferences are
-made from multiple individuals and/or multiple genotypes,</t>
-  </si>
-  <si>
-    <t>please create a separate table on this tab for each
-genotyope from which inferences are made, and cross-
-reference to separate genotype tables on the genotype tab.</t>
-  </si>
-  <si>
-    <t>Subject id:</t>
-  </si>
-  <si>
-    <t>Genotype id (as listed on the Genotype tab):</t>
+made from multiple individuals and/or multiple genotypes,
+please create a copy of the  table for each genotyope from
+which inferences are made, and cross-reference to separate
+genotype tables on the genotype tab. (see Notes tab for
+examples)</t>
+  </si>
+  <si>
+    <t>Subject id</t>
+  </si>
+  <si>
+    <t>Genotype id (as listed on the Genotype tab)</t>
   </si>
   <si>
     <t>sequence_id</t>
@@ -418,15 +416,18 @@
   </si>
   <si>
     <t>If inferences are made from multiple genotypes, please
-create separate tables for each genotype, and cross-
+create a copy of the table for each genotype, and cross-
 reference to the inferences made from each one on the
-Inferences tab.</t>
-  </si>
-  <si>
-    <t>Genotype Id:</t>
-  </si>
-  <si>
-    <t>Subject Id (as listed on Inferences tab):</t>
+Inferences tab. (see Notes tab for examples)</t>
+  </si>
+  <si>
+    <t>Genotype Id</t>
+  </si>
+  <si>
+    <t>Subject Id (as listed on Inferences tab)</t>
+  </si>
+  <si>
+    <t>Tool used to infer genotype</t>
   </si>
   <si>
     <t>subject_id</t>
@@ -479,6 +480,10 @@
 serttings used for this inference.</t>
   </si>
   <si>
+    <t>If multiple tools have been used, please create additional
+tables as needed.</t>
+  </si>
+  <si>
     <t>tool_name</t>
   </si>
   <si>
@@ -504,6 +509,64 @@
   <si>
     <t>Settings/configuration of the tool when used to provide the
 inferences (automatically generated)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>The submission should contain inferences derived from a single sequence dataset, detailed on the Repertoire tab. The
+dataset may contain sequences from more than one subject, in which case separate genotypes must be derived for each
+subject from which inferences are made. Species, and ethnicity, if provided, must be the same for all subjects for
+which inferences are submitted.</t>
+  </si>
+  <si>
+    <t>Sequence Numbering</t>
+  </si>
+  <si>
+    <t>Unless explicitly stated otherwise, all sequences should be numbered from 1 - that is, a sequence of length n should be numbered
+from 1 to n.</t>
+  </si>
+  <si>
+    <t>Output from Inference Tools</t>
+  </si>
+  <si>
+    <t>Inference tools authors have provided notes on the information that their tools can provide, which will be helpful in completing the
+Inferences and Genotype tabs. The notes are available from IARC on request.</t>
+  </si>
+  <si>
+    <t>Spreadsheet Structure</t>
+  </si>
+  <si>
+    <t>Your submission will be read into the IARC database automatically. To facilitate this, pleae don't make alterations to the layout or 
+structure of the workbook. In particular, please do not alter the positioning of tables, or the names of header fields.
+Some tables (e.g. Acknowledgements) may be extended as necessary - to do this, just insert additional rows into the table.</t>
+  </si>
+  <si>
+    <t>Inferences and Genotypes</t>
+  </si>
+  <si>
+    <t>You may submit inferences from multiple subjects and genotypes by duplicating the Subjects and Genotypes tables. 
+Some examples of typical scenarios may help:
+1. Inferences from a single subject, using a single tool from which you have derived a single genotype. 
+- In this case you could refer to the subject as Subject 1, and the genotype as Genotype 1. (you may use any 
+designations you wish, and may prefer to use more meaningful designations)
+- There would be a single Inference table and a single Genotype table. Both would be labelled Subject 1 and Genotype 1.
+2. Inferences from a single subject, using two inference tools. 
+- In this case there would be a single subject, say Subject 1, but two genotypes, say Genotype 1 and Genotype 2, one derived
+from each inference tool.
+- There would be two inference tables, one labelled Subject 1, Genotype 1 and one labelled Subject 1, Genotype 2. Each would 
+contain information derived from the corresponding tool and inferred genotype. Assuming that the same allele was inferred 
+from both genotypes, it would be present in both inference tables.
+- Likewise there would be two genotype tables, one labelled Subect 1, Genotype 1, and one labelled Subect 1, Genotype 2 
+3. Inferences from two subjects, using a single inference tool.
+- In this case there would be two subjects, say Subject 1 and Subject 2, and two genotypes, one for each subject, say Genotype 1
+and Genotype 2.
+- There would be two inference tables, one labelled Subject 1, Genotype 1 and one labelled Subject 2, Genotype 2.
+- Likewise there would be two Genotype tables, also labelled Subject 1, Genotype 1 and Subject 2, Genotype 2.</t>
+  </si>
+  <si>
+    <t>If more than one inference tool has been employed, please provide the genotypes inferred from each tool, as described above.
+In addition, please provide the settings used for each tool, by providing a table for each tool in the Tool Settings tab.</t>
   </si>
 </sst>
 </file>
@@ -547,7 +610,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -650,13 +713,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -665,9 +746,6 @@
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
     <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -675,11 +753,16 @@
     <xf borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,13 +1093,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4"/>
+    <row r="6" spans="1:4">
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="7" spans="1:4"/>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>1.3</v>
       </c>
     </row>
@@ -1024,126 +1111,126 @@
     <row r="10" spans="1:4"/>
     <row r="11" spans="1:4">
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4"/>
     <row r="13" spans="1:4">
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" s="6" t="s">
-        <v>8</v>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="B15" s="6" t="s">
-        <v>10</v>
+      <c r="B15" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="B16" s="6" t="s">
-        <v>12</v>
+      <c r="B16" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="B17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="B18" s="6" t="s">
-        <v>16</v>
+      <c r="B18" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="B19" s="6" t="s">
-        <v>18</v>
+      <c r="B19" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="B20" s="6" t="s">
-        <v>20</v>
+      <c r="B20" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="B21" s="6" t="s">
-        <v>22</v>
+      <c r="B21" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="B22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="B23" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>0</v>
@@ -1154,122 +1241,122 @@
     <row r="26" spans="1:4"/>
     <row r="27" spans="1:4">
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="B28" s="8" t="s">
-        <v>29</v>
+      <c r="B28" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:4"/>
     <row r="30" spans="1:4">
-      <c r="B30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="D30" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="8" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1288,39 +1375,39 @@
     <row r="42" spans="1:4"/>
     <row r="43" spans="1:4">
       <c r="B43" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="B44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C44" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="B45" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>34</v>
+      <c r="B45" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="B46" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>35</v>
+      <c r="B46" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:4"/>
@@ -1335,7 +1422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1353,170 +1440,159 @@
     <row r="2" spans="1:4"/>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="1" t="n"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5" s="8" t="s">
-        <v>38</v>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4"/>
     <row r="7" spans="1:4"/>
     <row r="8" spans="1:4">
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" s="6" t="s">
-        <v>41</v>
+      <c r="B10" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" s="6" t="s">
-        <v>45</v>
+      <c r="B12" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" s="6" t="s">
-        <v>47</v>
+      <c r="B13" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="B15" s="6" t="s">
-        <v>51</v>
+      <c r="B15" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="B16" s="6" t="s">
-        <v>53</v>
+      <c r="B16" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="B17" s="6" t="s">
-        <v>55</v>
+      <c r="B17" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="B18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="B19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="B20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1531,7 +1607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X50"/>
+  <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1572,182 +1648,110 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="B4" s="1" t="n"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
-      <c r="B6" s="8" t="s">
+    <row r="7" spans="1:24"/>
+    <row r="8" spans="1:24"/>
+    <row r="9" spans="1:24"/>
+    <row r="10" spans="1:24">
+      <c r="B10" s="14" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="B7" s="8" t="s">
+      <c r="C10" s="15" t="n"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="B11" s="14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:24"/>
-    <row r="9" spans="1:24">
-      <c r="B9" t="s">
+      <c r="C11" s="15" t="n"/>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="B12" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
-      <c r="B10" t="s">
+      <c r="C12" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
-      <c r="B11" s="3" t="s">
+      <c r="D12" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="H12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="I12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="J12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="K12" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="L12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="M12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="N12" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="O12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="P12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="Q12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="R12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="S12" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="T12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="U12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="W12" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="T11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="X11" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
-      <c r="B12" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R12" t="s">
-        <v>0</v>
-      </c>
-      <c r="S12" t="s">
-        <v>0</v>
-      </c>
-      <c r="T12" t="s">
-        <v>0</v>
-      </c>
-      <c r="U12" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12" t="s">
-        <v>0</v>
-      </c>
-      <c r="W12" t="s">
-        <v>0</v>
-      </c>
-      <c r="X12" s="7" t="s">
-        <v>0</v>
+      <c r="X12" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
@@ -1813,12 +1817,12 @@
       <c r="W13" t="s">
         <v>0</v>
       </c>
-      <c r="X13" s="7" t="s">
+      <c r="X13" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
@@ -1884,12 +1888,12 @@
       <c r="W14" t="s">
         <v>0</v>
       </c>
-      <c r="X14" s="7" t="s">
+      <c r="X14" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:24">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
@@ -1955,295 +1959,367 @@
       <c r="W15" t="s">
         <v>0</v>
       </c>
-      <c r="X15" s="7" t="s">
+      <c r="X15" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="B16" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="S16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="T16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="U16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="V16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="W16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="X16" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24"/>
+      <c r="B16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" t="s">
+        <v>0</v>
+      </c>
+      <c r="U16" t="s">
+        <v>0</v>
+      </c>
+      <c r="V16" t="s">
+        <v>0</v>
+      </c>
+      <c r="W16" t="s">
+        <v>0</v>
+      </c>
+      <c r="X16" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="B17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="V17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="18" spans="1:24"/>
     <row r="19" spans="1:24"/>
     <row r="20" spans="1:24"/>
     <row r="21" spans="1:24"/>
-    <row r="22" spans="1:24">
-      <c r="B22" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24"/>
-    <row r="24" spans="1:24">
-      <c r="B24" t="s">
-        <v>92</v>
-      </c>
-    </row>
+    <row r="22" spans="1:24"/>
+    <row r="23" spans="1:24">
+      <c r="B23" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24"/>
     <row r="25" spans="1:24">
       <c r="B25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="B26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24"/>
+    <row r="28" spans="1:24">
+      <c r="B28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="B29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="B30" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:24"/>
-    <row r="27" spans="1:24">
-      <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24">
-      <c r="B28" s="6" t="s">
+    <row r="31" spans="1:24">
+      <c r="B31" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C31" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
-      <c r="B29" s="6" t="s">
+    <row r="32" spans="1:24">
+      <c r="B32" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C32" s="16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
-      <c r="B30" s="6" t="s">
+    <row r="33" spans="1:24">
+      <c r="B33" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C33" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
-      <c r="B31" s="6" t="s">
+    <row r="34" spans="1:24">
+      <c r="B34" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C34" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
-      <c r="B32" s="6" t="s">
+    <row r="35" spans="1:24">
+      <c r="B35" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C35" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
-      <c r="B33" s="6" t="s">
+    <row r="36" spans="1:24">
+      <c r="B36" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C36" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
-      <c r="B34" s="6" t="s">
+    <row r="37" spans="1:24">
+      <c r="B37" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C37" s="16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
-      <c r="B35" s="6" t="s">
+    <row r="38" spans="1:24">
+      <c r="B38" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C38" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
-      <c r="B36" s="6" t="s">
+    <row r="39" spans="1:24">
+      <c r="B39" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C39" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
-      <c r="B37" s="6" t="s">
+    <row r="40" spans="1:24">
+      <c r="B40" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C40" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:24">
-      <c r="B38" s="6" t="s">
+    <row r="41" spans="1:24">
+      <c r="B41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C41" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
-      <c r="B39" s="6" t="s">
+    <row r="42" spans="1:24">
+      <c r="B42" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C42" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
-      <c r="B40" s="6" t="s">
+    <row r="43" spans="1:24">
+      <c r="B43" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C43" s="16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
-      <c r="B41" s="6" t="s">
+    <row r="44" spans="1:24">
+      <c r="B44" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C44" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
-      <c r="B42" s="6" t="s">
+    <row r="45" spans="1:24">
+      <c r="B45" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C45" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:24">
-      <c r="B43" s="6" t="s">
+    <row r="46" spans="1:24">
+      <c r="B46" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C46" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:24">
-      <c r="B44" s="6" t="s">
+    <row r="47" spans="1:24">
+      <c r="B47" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C47" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:24">
-      <c r="B45" s="6" t="s">
+    <row r="48" spans="1:24">
+      <c r="B48" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24">
+      <c r="B49" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
+      <c r="B50" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24">
-      <c r="B46" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24">
-      <c r="B47" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="14" t="s">
+      <c r="C50" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
-      <c r="B48" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24">
-      <c r="B49" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24">
-      <c r="B50" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="15" t="s">
+    <row r="51" spans="1:24">
+      <c r="B51" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
+      <c r="C51" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -2255,7 +2331,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T91"/>
+  <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2287,159 +2363,108 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:20"/>
     <row r="3" spans="1:20">
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="B4" s="1" t="n"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="B5" s="8" t="s">
-        <v>66</v>
+      <c r="B5" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="B6" s="8" t="s">
-        <v>118</v>
+      <c r="B6" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:20"/>
     <row r="8" spans="1:20">
-      <c r="B8" t="s">
+      <c r="B8" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="15" t="n"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="B9" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="15" t="n"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="B10" s="14" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="B9" t="s">
+      <c r="C10" s="15" t="n"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="B11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="B10" s="3" t="s">
+      <c r="D11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="H11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="I11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="J11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="K11" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="L11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="M11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="N11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="O11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="P11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="Q11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="R11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="S11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="T11" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="S10" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="B11" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" t="s">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>0</v>
-      </c>
-      <c r="S11" t="s">
-        <v>0</v>
-      </c>
-      <c r="T11" s="7" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
@@ -2493,12 +2518,12 @@
       <c r="S12" t="s">
         <v>0</v>
       </c>
-      <c r="T12" s="7" t="s">
+      <c r="T12" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
@@ -2552,12 +2577,12 @@
       <c r="S13" t="s">
         <v>0</v>
       </c>
-      <c r="T13" s="7" t="s">
+      <c r="T13" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
@@ -2611,12 +2636,12 @@
       <c r="S14" t="s">
         <v>0</v>
       </c>
-      <c r="T14" s="7" t="s">
+      <c r="T14" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
@@ -2670,12 +2695,12 @@
       <c r="S15" t="s">
         <v>0</v>
       </c>
-      <c r="T15" s="7" t="s">
+      <c r="T15" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
@@ -2729,12 +2754,12 @@
       <c r="S16" t="s">
         <v>0</v>
       </c>
-      <c r="T16" s="7" t="s">
+      <c r="T16" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C17" t="s">
@@ -2788,12 +2813,12 @@
       <c r="S17" t="s">
         <v>0</v>
       </c>
-      <c r="T17" s="7" t="s">
+      <c r="T17" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C18" t="s">
@@ -2847,12 +2872,12 @@
       <c r="S18" t="s">
         <v>0</v>
       </c>
-      <c r="T18" s="7" t="s">
+      <c r="T18" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:20">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C19" t="s">
@@ -2906,12 +2931,12 @@
       <c r="S19" t="s">
         <v>0</v>
       </c>
-      <c r="T19" s="7" t="s">
+      <c r="T19" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:20">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C20" t="s">
@@ -2965,12 +2990,12 @@
       <c r="S20" t="s">
         <v>0</v>
       </c>
-      <c r="T20" s="7" t="s">
+      <c r="T20" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:20">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C21" t="s">
@@ -3024,12 +3049,12 @@
       <c r="S21" t="s">
         <v>0</v>
       </c>
-      <c r="T21" s="7" t="s">
+      <c r="T21" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:20">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C22" t="s">
@@ -3083,12 +3108,12 @@
       <c r="S22" t="s">
         <v>0</v>
       </c>
-      <c r="T22" s="7" t="s">
+      <c r="T22" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:20">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C23" t="s">
@@ -3142,12 +3167,12 @@
       <c r="S23" t="s">
         <v>0</v>
       </c>
-      <c r="T23" s="7" t="s">
+      <c r="T23" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:20">
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C24" t="s">
@@ -3201,12 +3226,12 @@
       <c r="S24" t="s">
         <v>0</v>
       </c>
-      <c r="T24" s="7" t="s">
+      <c r="T24" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:20">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C25" t="s">
@@ -3260,12 +3285,12 @@
       <c r="S25" t="s">
         <v>0</v>
       </c>
-      <c r="T25" s="7" t="s">
+      <c r="T25" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C26" t="s">
@@ -3319,12 +3344,12 @@
       <c r="S26" t="s">
         <v>0</v>
       </c>
-      <c r="T26" s="7" t="s">
+      <c r="T26" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:20">
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C27" t="s">
@@ -3378,12 +3403,12 @@
       <c r="S27" t="s">
         <v>0</v>
       </c>
-      <c r="T27" s="7" t="s">
+      <c r="T27" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:20">
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C28" t="s">
@@ -3437,12 +3462,12 @@
       <c r="S28" t="s">
         <v>0</v>
       </c>
-      <c r="T28" s="7" t="s">
+      <c r="T28" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:20">
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C29" t="s">
@@ -3496,12 +3521,12 @@
       <c r="S29" t="s">
         <v>0</v>
       </c>
-      <c r="T29" s="7" t="s">
+      <c r="T29" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:20">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C30" t="s">
@@ -3555,12 +3580,12 @@
       <c r="S30" t="s">
         <v>0</v>
       </c>
-      <c r="T30" s="7" t="s">
+      <c r="T30" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:20">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C31" t="s">
@@ -3614,12 +3639,12 @@
       <c r="S31" t="s">
         <v>0</v>
       </c>
-      <c r="T31" s="7" t="s">
+      <c r="T31" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:20">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C32" t="s">
@@ -3673,12 +3698,12 @@
       <c r="S32" t="s">
         <v>0</v>
       </c>
-      <c r="T32" s="7" t="s">
+      <c r="T32" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:20">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C33" t="s">
@@ -3732,12 +3757,12 @@
       <c r="S33" t="s">
         <v>0</v>
       </c>
-      <c r="T33" s="7" t="s">
+      <c r="T33" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:20">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C34" t="s">
@@ -3791,12 +3816,12 @@
       <c r="S34" t="s">
         <v>0</v>
       </c>
-      <c r="T34" s="7" t="s">
+      <c r="T34" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:20">
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C35" t="s">
@@ -3850,12 +3875,12 @@
       <c r="S35" t="s">
         <v>0</v>
       </c>
-      <c r="T35" s="7" t="s">
+      <c r="T35" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:20">
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C36" t="s">
@@ -3909,12 +3934,12 @@
       <c r="S36" t="s">
         <v>0</v>
       </c>
-      <c r="T36" s="7" t="s">
+      <c r="T36" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:20">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C37" t="s">
@@ -3968,12 +3993,12 @@
       <c r="S37" t="s">
         <v>0</v>
       </c>
-      <c r="T37" s="7" t="s">
+      <c r="T37" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:20">
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C38" t="s">
@@ -4027,12 +4052,12 @@
       <c r="S38" t="s">
         <v>0</v>
       </c>
-      <c r="T38" s="7" t="s">
+      <c r="T38" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:20">
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C39" t="s">
@@ -4086,12 +4111,12 @@
       <c r="S39" t="s">
         <v>0</v>
       </c>
-      <c r="T39" s="7" t="s">
+      <c r="T39" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:20">
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C40" t="s">
@@ -4145,12 +4170,12 @@
       <c r="S40" t="s">
         <v>0</v>
       </c>
-      <c r="T40" s="7" t="s">
+      <c r="T40" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:20">
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C41" t="s">
@@ -4204,12 +4229,12 @@
       <c r="S41" t="s">
         <v>0</v>
       </c>
-      <c r="T41" s="7" t="s">
+      <c r="T41" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:20">
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C42" t="s">
@@ -4263,12 +4288,12 @@
       <c r="S42" t="s">
         <v>0</v>
       </c>
-      <c r="T42" s="7" t="s">
+      <c r="T42" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:20">
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C43" t="s">
@@ -4322,12 +4347,12 @@
       <c r="S43" t="s">
         <v>0</v>
       </c>
-      <c r="T43" s="7" t="s">
+      <c r="T43" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:20">
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C44" t="s">
@@ -4381,12 +4406,12 @@
       <c r="S44" t="s">
         <v>0</v>
       </c>
-      <c r="T44" s="7" t="s">
+      <c r="T44" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:20">
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C45" t="s">
@@ -4440,12 +4465,12 @@
       <c r="S45" t="s">
         <v>0</v>
       </c>
-      <c r="T45" s="7" t="s">
+      <c r="T45" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:20">
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C46" t="s">
@@ -4499,12 +4524,12 @@
       <c r="S46" t="s">
         <v>0</v>
       </c>
-      <c r="T46" s="7" t="s">
+      <c r="T46" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:20">
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C47" t="s">
@@ -4558,12 +4583,12 @@
       <c r="S47" t="s">
         <v>0</v>
       </c>
-      <c r="T47" s="7" t="s">
+      <c r="T47" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:20">
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C48" t="s">
@@ -4617,12 +4642,12 @@
       <c r="S48" t="s">
         <v>0</v>
       </c>
-      <c r="T48" s="7" t="s">
+      <c r="T48" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:20">
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C49" t="s">
@@ -4676,12 +4701,12 @@
       <c r="S49" t="s">
         <v>0</v>
       </c>
-      <c r="T49" s="7" t="s">
+      <c r="T49" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:20">
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C50" t="s">
@@ -4735,12 +4760,12 @@
       <c r="S50" t="s">
         <v>0</v>
       </c>
-      <c r="T50" s="7" t="s">
+      <c r="T50" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:20">
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C51" t="s">
@@ -4794,12 +4819,12 @@
       <c r="S51" t="s">
         <v>0</v>
       </c>
-      <c r="T51" s="7" t="s">
+      <c r="T51" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:20">
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C52" t="s">
@@ -4853,12 +4878,12 @@
       <c r="S52" t="s">
         <v>0</v>
       </c>
-      <c r="T52" s="7" t="s">
+      <c r="T52" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:20">
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C53" t="s">
@@ -4912,12 +4937,12 @@
       <c r="S53" t="s">
         <v>0</v>
       </c>
-      <c r="T53" s="7" t="s">
+      <c r="T53" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:20">
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C54" t="s">
@@ -4971,12 +4996,12 @@
       <c r="S54" t="s">
         <v>0</v>
       </c>
-      <c r="T54" s="7" t="s">
+      <c r="T54" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:20">
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C55" t="s">
@@ -5030,12 +5055,12 @@
       <c r="S55" t="s">
         <v>0</v>
       </c>
-      <c r="T55" s="7" t="s">
+      <c r="T55" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:20">
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C56" t="s">
@@ -5089,12 +5114,12 @@
       <c r="S56" t="s">
         <v>0</v>
       </c>
-      <c r="T56" s="7" t="s">
+      <c r="T56" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:20">
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C57" t="s">
@@ -5148,12 +5173,12 @@
       <c r="S57" t="s">
         <v>0</v>
       </c>
-      <c r="T57" s="7" t="s">
+      <c r="T57" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:20">
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C58" t="s">
@@ -5207,12 +5232,12 @@
       <c r="S58" t="s">
         <v>0</v>
       </c>
-      <c r="T58" s="7" t="s">
+      <c r="T58" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:20">
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C59" t="s">
@@ -5266,258 +5291,318 @@
       <c r="S59" t="s">
         <v>0</v>
       </c>
-      <c r="T59" s="7" t="s">
+      <c r="T59" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:20">
-      <c r="B60" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="S60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="T60" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20"/>
+      <c r="B60" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>0</v>
+      </c>
+      <c r="G60" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" t="s">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
+        <v>0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>0</v>
+      </c>
+      <c r="K60" t="s">
+        <v>0</v>
+      </c>
+      <c r="L60" t="s">
+        <v>0</v>
+      </c>
+      <c r="M60" t="s">
+        <v>0</v>
+      </c>
+      <c r="N60" t="s">
+        <v>0</v>
+      </c>
+      <c r="O60" t="s">
+        <v>0</v>
+      </c>
+      <c r="P60" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>0</v>
+      </c>
+      <c r="R60" t="s">
+        <v>0</v>
+      </c>
+      <c r="S60" t="s">
+        <v>0</v>
+      </c>
+      <c r="T60" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
+      <c r="B61" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T61" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="62" spans="1:20"/>
     <row r="63" spans="1:20"/>
     <row r="64" spans="1:20"/>
     <row r="65" spans="1:20"/>
-    <row r="66" spans="1:20">
-      <c r="B66" s="1" t="s">
+    <row r="66" spans="1:20"/>
+    <row r="67" spans="1:20">
+      <c r="B67" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
+      <c r="B68" s="1" t="n"/>
+    </row>
+    <row r="69" spans="1:20">
+      <c r="B69" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
-      <c r="B67" s="1" t="n"/>
-    </row>
-    <row r="68" spans="1:20">
-      <c r="B68" t="s">
+    <row r="70" spans="1:20">
+      <c r="B70" s="13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
-      <c r="B69" s="13" t="s">
+    <row r="71" spans="1:20">
+      <c r="B71" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20"/>
+    <row r="73" spans="1:20">
+      <c r="B73" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
+      <c r="B74" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C74" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
-      <c r="B70" t="s">
+    <row r="75" spans="1:20">
+      <c r="B75" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
+      <c r="B76" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:20"/>
-    <row r="72" spans="1:20">
-      <c r="B72" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20">
-      <c r="B73" s="6" t="s">
+    <row r="77" spans="1:20">
+      <c r="B77" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20">
-      <c r="B74" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" s="14" t="s">
+      <c r="C77" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="1:20">
-      <c r="B75" s="6" t="s">
+    <row r="78" spans="1:20">
+      <c r="B78" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20">
-      <c r="B76" s="6" t="s">
+      <c r="C78" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
+      <c r="B79" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20">
-      <c r="B77" s="6" t="s">
+      <c r="C79" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
+      <c r="B80" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20">
-      <c r="B78" s="6" t="s">
+      <c r="C80" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
+      <c r="B81" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C81" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:20">
-      <c r="B79" s="6" t="s">
+    <row r="82" spans="1:20">
+      <c r="B82" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C82" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:20">
-      <c r="B80" s="6" t="s">
+    <row r="83" spans="1:20">
+      <c r="B83" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20">
-      <c r="B81" s="6" t="s">
+      <c r="C83" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
+      <c r="B84" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="14" t="s">
+      <c r="C84" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
-      <c r="B82" s="6" t="s">
+    <row r="85" spans="1:20">
+      <c r="B85" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="14" t="s">
+      <c r="C85" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="83" spans="1:20">
-      <c r="B83" s="6" t="s">
+    <row r="86" spans="1:20">
+      <c r="B86" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C86" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="84" spans="1:20">
-      <c r="B84" s="6" t="s">
+    <row r="87" spans="1:20">
+      <c r="B87" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C87" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:20">
-      <c r="B85" s="6" t="s">
+    <row r="88" spans="1:20">
+      <c r="B88" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C88" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="86" spans="1:20">
-      <c r="B86" s="6" t="s">
+    <row r="89" spans="1:20">
+      <c r="B89" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C89" s="16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:20">
-      <c r="B87" s="6" t="s">
+    <row r="90" spans="1:20">
+      <c r="B90" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C90" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:20">
-      <c r="B88" s="6" t="s">
+    <row r="91" spans="1:20">
+      <c r="B91" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="14" t="s">
+      <c r="C91" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="89" spans="1:20">
-      <c r="B89" s="6" t="s">
+    <row r="92" spans="1:20">
+      <c r="B92" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="14" t="s">
+      <c r="C92" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:20">
-      <c r="B90" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="91" spans="1:20">
-      <c r="B91" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
+    <row r="93" spans="1:20"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -5529,7 +5614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5538,7 +5623,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="2"/>
-    <col customWidth="1" max="2" min="2" width="57"/>
+    <col customWidth="1" max="2" min="2" width="60"/>
     <col customWidth="1" max="3" min="3" width="61"/>
     <col customWidth="1" max="4" min="4" width="10"/>
   </cols>
@@ -5547,78 +5632,178 @@
     <row r="2" spans="1:4"/>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4"/>
     <row r="5" spans="1:4">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:4"/>
-    <row r="7" spans="1:4">
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
+    <row r="7" spans="1:4"/>
+    <row r="8" spans="1:4">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="6" t="s">
+      <c r="D9" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" s="6" t="s">
+      <c r="D10" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C11" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="9" t="s">
+      <c r="D11" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4"/>
+      <c r="D12" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="13" spans="1:4"/>
     <row r="14" spans="1:4"/>
     <row r="15" spans="1:4"/>
     <row r="16" spans="1:4"/>
-    <row r="17" spans="1:4">
-      <c r="B17" s="1" t="n"/>
+    <row r="17" spans="1:4"/>
+    <row r="18" spans="1:4">
+      <c r="B18" s="1" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="2"/>
+    <col customWidth="1" max="2" min="2" width="135"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2"/>
+    <row r="2" spans="1:2">
+      <c r="B2" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2"/>
+    <row r="4" spans="1:2">
+      <c r="B4" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2"/>
+    <row r="7" spans="1:2">
+      <c r="B7" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2"/>
+    <row r="10" spans="1:2">
+      <c r="B10" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2"/>
+    <row r="13" spans="1:2">
+      <c r="B13" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2"/>
+    <row r="16" spans="1:2">
+      <c r="B16" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2"/>
+    <row r="19" spans="1:2">
+      <c r="B19" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Minor changes to clarify use of public repositories
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="154">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -160,7 +160,8 @@
     <t>repository_name</t>
   </si>
   <si>
-    <t>Name of the repository holding the sequence dataset</t>
+    <t>Name of the repository holding the sequence dataset (e.g.
+NIH SRA)</t>
   </si>
   <si>
     <t>repository_id</t>
@@ -173,20 +174,22 @@
     <t>dataset_url</t>
   </si>
   <si>
-    <t>URL of the sequence dataset (if any)</t>
+    <t>URL of the sequence dataset (in the case of the NIH SRA,
+please provide the URL to the Project)</t>
   </si>
   <si>
     <t>dataset_doi</t>
   </si>
   <si>
-    <t>doi of the sequence dataset (if any)</t>
+    <t>doi of the sequence dataset (If any. Not all archives
+provide a doi, in particular the NIH SRA does not)</t>
   </si>
   <si>
     <t>miarr_compliant</t>
   </si>
   <si>
-    <t>TRUE if the repertoire dataset and associated metadata is in
-MiAIRR format</t>
+    <t>TRUE if the repertoire dataset and associated metadata is
+available in MiAIRR format</t>
   </si>
   <si>
     <t>miairr_link</t>
@@ -219,6 +222,13 @@
   <si>
     <t>sequences of reverse pcr primers used for sequence
 amplification</t>
+  </si>
+  <si>
+    <t>primers_not_overlapping</t>
+  </si>
+  <si>
+    <t>Please confirm that primers do not overlap with the stated
+sequence of any inferred allele.</t>
   </si>
   <si>
     <t>notes</t>
@@ -345,7 +355,7 @@
   </si>
   <si>
     <t>List of nucleotide substitutions (e.g. G112A) between this
-sequence and the closest reference gene and allele</t>
+sequence and the closest reference gene and allele.</t>
   </si>
   <si>
     <t>Number of amino acids that differ between this sequence and
@@ -353,31 +363,34 @@
   </si>
   <si>
     <t>List of amino acid substitutions (e.g. A96N) between this
-sequence and the closest reference gene and allele</t>
-  </si>
-  <si>
-    <t>The proportion of records in the sequence dataset matching
-this unmutated sequence</t>
+sequence and the closest reference gene and allele. Please
+use IMGT numbering for V-genes, and number from start of
+coding sequence for D- or J- genes.</t>
+  </si>
+  <si>
+    <t>The proportion of unmutated sequences in the dataset
+represented by this sequence.</t>
   </si>
   <si>
     <t>The number of records in the sequence dataset exactly
 matching this unmutated sequence</t>
   </si>
   <si>
-    <t>The number of molecules (identified by UMIs) exactly
-matching this unmutated sequence</t>
+    <t>The number of molecules (identified by Unique Molecular
+Identifiers) exactly matching this unmutated sequence (if
+UMIs were used)</t>
   </si>
   <si>
     <t>The percentage at which this allele was observed in the
 sequence dataset, compared to other alleles</t>
   </si>
   <si>
-    <t>Number of unique D sequences found associated with the
-inferred V sequence</t>
-  </si>
-  <si>
-    <t>Number of unique J sequences found associated with the
-inferred V sequence</t>
+    <t>Number of D allele calls (i.e., unique allelic sequences)
+found associated with an inferred V sequence</t>
+  </si>
+  <si>
+    <t>Number of J allele calls (i.e., unique allelic sequences)
+found associated with an inferred V sequence</t>
   </si>
   <si>
     <t>Number of unique CDR3s found associated with the inferred V
@@ -460,9 +473,17 @@
 allele</t>
   </si>
   <si>
+    <t>List of nucleotide substitutions (e.g. G112A) between this
+sequence and the closest reference gene and allele</t>
+  </si>
+  <si>
     <t>For inferred alleles, the number of amino acids that differ
 between this sequence and the closest reference gene and
 allele</t>
+  </si>
+  <si>
+    <t>Number of unique CDR3s found associated with an inferred V
+sequence</t>
   </si>
   <si>
     <t>Tool Settings</t>
@@ -1064,7 +1085,7 @@
     <col customWidth="1" max="1" min="1" width="3"/>
     <col customWidth="1" max="2" min="2" width="61"/>
     <col customWidth="1" max="3" min="3" width="62"/>
-    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="4" min="4" width="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4"/>
@@ -1414,7 +1435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1425,7 +1446,7 @@
     <col customWidth="1" max="1" min="1" width="2"/>
     <col customWidth="1" max="2" min="2" width="55"/>
     <col customWidth="1" max="3" min="3" width="62"/>
-    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="4" min="4" width="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4"/>
@@ -1471,7 +1492,7 @@
       <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -1493,7 +1514,7 @@
       <c r="B12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1504,7 +1525,7 @@
       <c r="B13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -1578,13 +1599,24 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1610,7 +1642,7 @@
     <col customWidth="1" max="1" min="1" width="3"/>
     <col customWidth="1" max="2" min="2" width="62"/>
     <col customWidth="1" max="3" min="3" width="62"/>
-    <col customWidth="1" max="4" min="4" width="19"/>
+    <col customWidth="1" max="4" min="4" width="50"/>
     <col customWidth="1" max="5" min="5" width="14"/>
     <col customWidth="1" max="6" min="6" width="9"/>
     <col customWidth="1" max="7" min="7" width="18"/>
@@ -1640,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -1648,12 +1680,12 @@
     </row>
     <row r="5" spans="1:24">
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:24"/>
@@ -1661,73 +1693,73 @@
     <row r="9" spans="1:24"/>
     <row r="10" spans="1:24">
       <c r="B10" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10" s="15" t="n"/>
     </row>
     <row r="11" spans="1:24">
       <c r="B11" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C11" s="15" t="n"/>
     </row>
     <row r="12" spans="1:24">
       <c r="B12" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="U12" s="5" t="s">
         <v>42</v>
@@ -1736,7 +1768,7 @@
         <v>44</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="X12" s="6" t="s">
         <v>27</v>
@@ -2104,18 +2136,18 @@
     <row r="22" spans="1:24"/>
     <row r="23" spans="1:24">
       <c r="B23" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:24"/>
     <row r="25" spans="1:24">
       <c r="B25" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:24">
       <c r="B26" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:24"/>
@@ -2129,154 +2161,154 @@
     </row>
     <row r="29" spans="1:24">
       <c r="B29" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:24">
       <c r="B30" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:24">
       <c r="B31" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:24">
       <c r="B32" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:24">
       <c r="B33" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:24">
       <c r="B34" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:24">
       <c r="B35" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:24">
       <c r="B36" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:24">
       <c r="B37" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:24">
       <c r="B38" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="B39" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:24">
       <c r="B40" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:24">
       <c r="B41" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:24">
       <c r="B42" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:24">
       <c r="B43" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:24">
       <c r="B44" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:24">
       <c r="B45" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:24">
       <c r="B46" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:24">
       <c r="B47" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:24">
@@ -2284,7 +2316,7 @@
         <v>42</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:24">
@@ -2292,15 +2324,15 @@
         <v>44</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:24">
       <c r="B50" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:24">
@@ -2334,7 +2366,7 @@
     <col customWidth="1" max="1" min="1" width="4"/>
     <col customWidth="1" max="2" min="2" width="62"/>
     <col customWidth="1" max="3" min="3" width="62"/>
-    <col customWidth="1" max="4" min="4" width="19"/>
+    <col customWidth="1" max="4" min="4" width="50"/>
     <col customWidth="1" max="5" min="5" width="14"/>
     <col customWidth="1" max="6" min="6" width="9"/>
     <col customWidth="1" max="7" min="7" width="18"/>
@@ -2354,13 +2386,13 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:19"/>
     <row r="3" spans="1:19">
       <c r="B3" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2368,87 +2400,87 @@
     </row>
     <row r="5" spans="1:19">
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="B6" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:19"/>
     <row r="8" spans="1:19">
       <c r="B8" s="14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C8" s="15" t="n"/>
     </row>
     <row r="9" spans="1:19">
       <c r="B9" s="14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C9" s="15" t="n"/>
     </row>
     <row r="10" spans="1:19">
       <c r="B10" s="14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C10" s="15" t="n"/>
     </row>
     <row r="11" spans="1:19">
       <c r="B11" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -5258,7 +5290,7 @@
     <row r="66" spans="1:19"/>
     <row r="67" spans="1:19">
       <c r="B67" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:19">
@@ -5266,17 +5298,17 @@
     </row>
     <row r="69" spans="1:19">
       <c r="B69" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:19">
       <c r="B70" s="13" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:19">
       <c r="B71" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:19"/>
@@ -5290,146 +5322,146 @@
     </row>
     <row r="74" spans="1:19">
       <c r="B74" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:19">
       <c r="B75" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:19">
       <c r="B76" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="77" spans="1:19">
       <c r="B77" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:19">
       <c r="B78" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:19">
       <c r="B79" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:19">
       <c r="B80" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:19">
       <c r="B81" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:19">
       <c r="B82" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:19">
       <c r="B83" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:19">
       <c r="B84" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:19">
       <c r="B85" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:19">
       <c r="B86" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:19">
       <c r="B87" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:19">
       <c r="B88" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="1:19">
       <c r="B89" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:19">
       <c r="B90" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:19">
       <c r="B91" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:19"/>
@@ -5455,25 +5487,25 @@
     <col customWidth="1" max="1" min="1" width="2"/>
     <col customWidth="1" max="2" min="2" width="60"/>
     <col customWidth="1" max="3" min="3" width="61"/>
-    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="4" min="4" width="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4"/>
     <row r="2" spans="1:4"/>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4"/>
     <row r="5" spans="1:4">
       <c r="B5" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:4"/>
@@ -5490,10 +5522,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>0</v>
@@ -5501,10 +5533,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>0</v>
@@ -5512,10 +5544,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="7" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>0</v>
@@ -5523,10 +5555,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>0</v>
@@ -5566,7 +5598,7 @@
     <row r="1" spans="1:2"/>
     <row r="2" spans="1:2">
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2"/>
@@ -5577,62 +5609,62 @@
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2"/>
     <row r="7" spans="1:2">
       <c r="B7" s="13" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="18" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:2"/>
     <row r="10" spans="1:2">
       <c r="B10" s="13" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:2"/>
     <row r="13" spans="1:2">
       <c r="B13" s="13" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:2"/>
     <row r="16" spans="1:2">
       <c r="B16" s="13" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="B17" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:2"/>
     <row r="19" spans="1:2">
       <c r="B19" s="13" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates following review at IARC meeting 26/6
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -1102,12 +1102,12 @@
       <c r="B4" s="1" t="n"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="C5" t="s">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="9" spans="1:4"/>

</xml_diff>

<commit_message>
Added / modified accession numbers to match the defined approach with NIH Modified descriptions for allelic percentages to clarify their calculation
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="158">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -161,28 +161,20 @@
   </si>
   <si>
     <t>Name of the repository holding the sequence dataset (e.g.
-NIH SRA)</t>
+NIH SRA, or ENA)</t>
   </si>
   <si>
     <t>repository_id</t>
   </si>
   <si>
-    <t>Id or serial number of the sequence dataset within the
-repository</t>
+    <t>Accession number or serial number within the repository
+(e.g. NIH Project or ENA Study)</t>
   </si>
   <si>
     <t>dataset_url</t>
   </si>
   <si>
-    <t>URL of the sequence dataset (in the case of the NIH SRA,
-please provide the URL to the Project)</t>
-  </si>
-  <si>
-    <t>dataset_doi</t>
-  </si>
-  <si>
-    <t>doi of the sequence dataset (If any. Not all archives
-provide a doi, in particular the NIH SRA does not)</t>
+    <t>URL of the study or project within the repository</t>
   </si>
   <si>
     <t>miarr_compliant</t>
@@ -263,10 +255,16 @@
     <t>Genotype id (as listed on the Genotype tab)</t>
   </si>
   <si>
+    <t>Run Id(s)</t>
+  </si>
+  <si>
     <t>sequence_id</t>
   </si>
   <si>
     <t>sequences</t>
+  </si>
+  <si>
+    <t>domain</t>
   </si>
   <si>
     <t>closest_reference</t>
@@ -328,18 +326,31 @@
   <si>
     <t>'Number of sequences': where sequences are counted the count
 should be conducted after quality control  UMI processing
-and replicate/error cloud removal.</t>
+and replicate/error cloud removal (where these are used).</t>
   </si>
   <si>
     <t>'Reference genes and alleles' - this is the set of genes and
 alleles provided to the inference tool.</t>
   </si>
   <si>
+    <t>Subject Id' should be assigned by the submitter, to
+differentiate between different subjects from which
+inferences are made in this submission</t>
+  </si>
+  <si>
+    <t>Run Id(s)'  should list the accession numbers of sequence
+sets in the repository (e.g. NIH SRA or ENA) listing the raw
+sequences from which this inference was made</t>
+  </si>
+  <si>
     <t>Identifier of the allele, issued by the submitter (need not
 follow any particular format)</t>
   </si>
   <si>
     <t>Overall number of sequences assigned to this allele</t>
+  </si>
+  <si>
+    <t>Sequence domain (V, D, J or Constant)</t>
   </si>
   <si>
     <t>The closest reference gene and allele, as inferred by the
@@ -368,12 +379,13 @@
 coding sequence for D- or J- genes.</t>
   </si>
   <si>
-    <t>The proportion of unmutated sequences in the dataset
-represented by this sequence.</t>
-  </si>
-  <si>
-    <t>The number of records in the sequence dataset exactly
-matching this unmutated sequence</t>
+    <t>The number of sequences exactly matching the sequence of
+this allele divided by the number of sequences exactly
+matching any allele of any gene, *100</t>
+  </si>
+  <si>
+    <t>The number of sequences exactly matching this unmutated
+sequence</t>
   </si>
   <si>
     <t>The number of molecules (identified by Unique Molecular
@@ -381,8 +393,9 @@
 UMIs were used)</t>
   </si>
   <si>
-    <t>The percentage at which this allele was observed in the
-sequence dataset, compared to other alleles</t>
+    <t>The number of sequences exactly matching the sequence of
+this allele divided by the number of sequences exactly
+matching any allele of this specific gene, *100</t>
   </si>
   <si>
     <t>Number of D allele calls (i.e., unique allelic sequences)
@@ -437,6 +450,9 @@
     <t>Genotype Id</t>
   </si>
   <si>
+    <t>Biosample Id(s)</t>
+  </si>
+  <si>
     <t>Subject Id (as listed on Inferences tab)</t>
   </si>
   <si>
@@ -448,11 +464,12 @@
   <si>
     <t>'Number of sequences': where sequences are counted the count
 should be conducted after quality control UMI processing and
-replicate/error cloud removal.</t>
-  </si>
-  <si>
-    <t>Question for review - should this be the number of distinct
-sequences  or a molecule count?</t>
+replicate/error cloud removal (where these are used).</t>
+  </si>
+  <si>
+    <t>Biosample Id(s)'  should list the accession numbers of
+samples from which this genotype was inferred  (e.g. NIH
+biosamples or ENA samples)</t>
   </si>
   <si>
     <t>Identifier of the allele (either IMGT, or the name assigned
@@ -1435,7 +1452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1514,7 +1531,7 @@
       <c r="B12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1536,7 +1553,7 @@
       <c r="B14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>51</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -1569,7 +1586,7 @@
       <c r="B17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="8" t="s">
@@ -1599,24 +1616,13 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1631,7 +1637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X52"/>
+  <dimension ref="A1:Y56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1643,209 +1649,148 @@
     <col customWidth="1" max="2" min="2" width="62"/>
     <col customWidth="1" max="3" min="3" width="62"/>
     <col customWidth="1" max="4" min="4" width="50"/>
-    <col customWidth="1" max="5" min="5" width="14"/>
-    <col customWidth="1" max="6" min="6" width="9"/>
-    <col customWidth="1" max="7" min="7" width="18"/>
-    <col customWidth="1" max="8" min="8" width="9"/>
-    <col customWidth="1" max="9" min="9" width="18"/>
-    <col customWidth="1" max="10" min="10" width="21"/>
+    <col customWidth="1" max="5" min="5" width="19"/>
+    <col customWidth="1" max="6" min="6" width="14"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="18"/>
+    <col customWidth="1" max="9" min="9" width="9"/>
+    <col customWidth="1" max="10" min="10" width="18"/>
     <col customWidth="1" max="11" min="11" width="21"/>
-    <col customWidth="1" max="12" min="12" width="16"/>
-    <col customWidth="1" max="13" min="13" width="20"/>
-    <col customWidth="1" max="14" min="14" width="11"/>
+    <col customWidth="1" max="12" min="12" width="21"/>
+    <col customWidth="1" max="13" min="13" width="16"/>
+    <col customWidth="1" max="14" min="14" width="20"/>
     <col customWidth="1" max="15" min="15" width="11"/>
-    <col customWidth="1" max="16" min="16" width="14"/>
-    <col customWidth="1" max="17" min="17" width="19"/>
+    <col customWidth="1" max="16" min="16" width="11"/>
+    <col customWidth="1" max="17" min="17" width="14"/>
     <col customWidth="1" max="18" min="18" width="19"/>
-    <col customWidth="1" max="19" min="19" width="13"/>
+    <col customWidth="1" max="19" min="19" width="19"/>
     <col customWidth="1" max="20" min="20" width="13"/>
-    <col customWidth="1" max="21" min="21" width="17"/>
-    <col customWidth="1" max="22" min="22" width="15"/>
-    <col customWidth="1" max="23" min="23" width="19"/>
-    <col customWidth="1" max="24" min="24" width="15"/>
+    <col customWidth="1" max="21" min="21" width="13"/>
+    <col customWidth="1" max="22" min="22" width="17"/>
+    <col customWidth="1" max="23" min="23" width="15"/>
+    <col customWidth="1" max="24" min="24" width="19"/>
+    <col customWidth="1" max="25" min="25" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24"/>
-    <row r="2" spans="1:24"/>
-    <row r="3" spans="1:24">
+    <row r="1" spans="1:25"/>
+    <row r="2" spans="1:25"/>
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="B4" s="1" t="n"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="B5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
-      <c r="B4" s="1" t="n"/>
-    </row>
-    <row r="5" spans="1:24">
-      <c r="B5" s="2" t="s">
+    <row r="7" spans="1:25"/>
+    <row r="8" spans="1:25"/>
+    <row r="9" spans="1:25"/>
+    <row r="10" spans="1:25">
+      <c r="B10" s="14" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="B6" s="2" t="s">
+      <c r="C10" s="15" t="n"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="B11" s="14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:24"/>
-    <row r="8" spans="1:24"/>
-    <row r="9" spans="1:24"/>
-    <row r="10" spans="1:24">
-      <c r="B10" s="14" t="s">
+      <c r="C11" s="15" t="n"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="B12" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="15" t="n"/>
-    </row>
-    <row r="11" spans="1:24">
-      <c r="B11" s="14" t="s">
+      <c r="C12" s="15" t="n"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="B13" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="15" t="n"/>
-    </row>
-    <row r="12" spans="1:24">
-      <c r="B12" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="P13" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="P12" s="5" t="s">
+      <c r="Q13" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="R13" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="S13" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="S12" s="5" t="s">
+      <c r="T13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="T12" s="5" t="s">
+      <c r="U13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="V13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="V12" s="5" t="s">
+      <c r="W13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="W12" s="5" t="s">
+      <c r="X13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="X12" s="6" t="s">
+      <c r="Y13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
-      <c r="B13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
-        <v>0</v>
-      </c>
-      <c r="L13" t="s">
-        <v>0</v>
-      </c>
-      <c r="M13" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>0</v>
-      </c>
-      <c r="R13" t="s">
-        <v>0</v>
-      </c>
-      <c r="S13" t="s">
-        <v>0</v>
-      </c>
-      <c r="T13" t="s">
-        <v>0</v>
-      </c>
-      <c r="U13" t="s">
-        <v>0</v>
-      </c>
-      <c r="V13" t="s">
-        <v>0</v>
-      </c>
-      <c r="W13" t="s">
-        <v>0</v>
-      </c>
-      <c r="X13" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:25">
       <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
@@ -1912,11 +1857,14 @@
       <c r="W14" t="s">
         <v>0</v>
       </c>
-      <c r="X14" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="X14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
       <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
@@ -1983,11 +1931,14 @@
       <c r="W15" t="s">
         <v>0</v>
       </c>
-      <c r="X15" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="X15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="B16" s="7" t="s">
         <v>0</v>
       </c>
@@ -2054,296 +2005,394 @@
       <c r="W16" t="s">
         <v>0</v>
       </c>
-      <c r="X16" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="B17" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="S17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="T17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="U17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="V17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="W17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="X17" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24"/>
-    <row r="19" spans="1:24"/>
-    <row r="20" spans="1:24"/>
-    <row r="21" spans="1:24"/>
-    <row r="22" spans="1:24"/>
-    <row r="23" spans="1:24">
-      <c r="B23" s="1" t="s">
+      <c r="X16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="B17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>0</v>
+      </c>
+      <c r="V17" t="s">
+        <v>0</v>
+      </c>
+      <c r="W17" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="B18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="V18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="X18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25"/>
+    <row r="20" spans="1:25"/>
+    <row r="21" spans="1:25"/>
+    <row r="22" spans="1:25"/>
+    <row r="23" spans="1:25"/>
+    <row r="24" spans="1:25">
+      <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:24"/>
-    <row r="25" spans="1:24">
-      <c r="B25" t="s">
+    <row r="25" spans="1:25"/>
+    <row r="26" spans="1:25">
+      <c r="B26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
-      <c r="B26" t="s">
+    <row r="27" spans="1:25">
+      <c r="B27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:24"/>
-    <row r="28" spans="1:24">
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="1:25">
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25"/>
+    <row r="31" spans="1:25">
+      <c r="B31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
-      <c r="B29" s="7" t="s">
+    <row r="32" spans="1:25">
+      <c r="B32" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="B33" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24">
-      <c r="B30" s="7" t="s">
+      <c r="C33" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="B34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24">
-      <c r="B31" s="7" t="s">
+      <c r="C34" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="B35" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24">
-      <c r="B32" s="7" t="s">
+      <c r="C35" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="B36" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24">
-      <c r="B33" s="7" t="s">
+      <c r="C36" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="B37" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24">
-      <c r="B34" s="7" t="s">
+      <c r="C37" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
+      <c r="B38" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24">
-      <c r="B35" s="7" t="s">
+      <c r="C38" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="B39" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24">
-      <c r="B36" s="7" t="s">
+      <c r="C39" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="B40" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24">
-      <c r="B37" s="7" t="s">
+      <c r="C40" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="B41" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24">
-      <c r="B38" s="7" t="s">
+      <c r="C41" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="B42" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24">
-      <c r="B39" s="7" t="s">
+      <c r="C42" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
+      <c r="B43" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24">
-      <c r="B40" s="7" t="s">
+      <c r="C43" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
+      <c r="B44" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24">
-      <c r="B41" s="7" t="s">
+      <c r="C44" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
+      <c r="B45" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24">
-      <c r="B42" s="7" t="s">
+      <c r="C45" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25">
+      <c r="B46" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24">
-      <c r="B43" s="7" t="s">
+      <c r="C46" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
+      <c r="B47" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24">
-      <c r="B44" s="7" t="s">
+      <c r="C47" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25">
+      <c r="B48" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24">
-      <c r="B45" s="7" t="s">
+      <c r="C48" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25">
+      <c r="B49" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24">
-      <c r="B46" s="7" t="s">
+      <c r="C49" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25">
+      <c r="B50" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24">
-      <c r="B47" s="7" t="s">
+      <c r="C50" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25">
+      <c r="B51" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24">
-      <c r="B48" s="7" t="s">
+      <c r="C51" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25">
+      <c r="B52" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24">
-      <c r="B49" s="7" t="s">
+      <c r="C52" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25">
+      <c r="B53" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24">
-      <c r="B50" s="7" t="s">
+      <c r="C53" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25">
+      <c r="B54" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24">
-      <c r="B51" s="9" t="s">
+      <c r="C54" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25">
+      <c r="B55" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C55" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:24"/>
+    <row r="56" spans="1:25"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -2355,7 +2404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S92"/>
+  <dimension ref="A1:S94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2386,13 +2435,13 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:19"/>
     <row r="3" spans="1:19">
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2400,143 +2449,93 @@
     </row>
     <row r="5" spans="1:19">
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="B6" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:19"/>
     <row r="8" spans="1:19">
       <c r="B8" s="14" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C8" s="15" t="n"/>
     </row>
     <row r="9" spans="1:19">
       <c r="B9" s="14" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C9" s="15" t="n"/>
     </row>
     <row r="10" spans="1:19">
       <c r="B10" s="14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C10" s="15" t="n"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="15" t="n"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="B12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="P12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="Q12" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="R11" s="5" t="s">
+      <c r="R12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="S11" s="6" t="s">
+      <c r="S12" s="6" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="B12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R12" t="s">
-        <v>0</v>
-      </c>
-      <c r="S12" s="8" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -5228,82 +5227,133 @@
       </c>
     </row>
     <row r="61" spans="1:19">
-      <c r="B61" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R61" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="S61" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19"/>
+      <c r="B61" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>0</v>
+      </c>
+      <c r="G61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H61" t="s">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>0</v>
+      </c>
+      <c r="J61" t="s">
+        <v>0</v>
+      </c>
+      <c r="K61" t="s">
+        <v>0</v>
+      </c>
+      <c r="L61" t="s">
+        <v>0</v>
+      </c>
+      <c r="M61" t="s">
+        <v>0</v>
+      </c>
+      <c r="N61" t="s">
+        <v>0</v>
+      </c>
+      <c r="O61" t="s">
+        <v>0</v>
+      </c>
+      <c r="P61" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>0</v>
+      </c>
+      <c r="R61" t="s">
+        <v>0</v>
+      </c>
+      <c r="S61" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
+      <c r="B62" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S62" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="63" spans="1:19"/>
     <row r="64" spans="1:19"/>
     <row r="65" spans="1:19"/>
     <row r="66" spans="1:19"/>
-    <row r="67" spans="1:19">
-      <c r="B67" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
+    <row r="67" spans="1:19"/>
     <row r="68" spans="1:19">
-      <c r="B68" s="1" t="n"/>
+      <c r="B68" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="69" spans="1:19">
-      <c r="B69" t="s">
-        <v>123</v>
-      </c>
+      <c r="B69" s="1" t="n"/>
     </row>
     <row r="70" spans="1:19">
-      <c r="B70" s="13" t="s">
-        <v>124</v>
+      <c r="B70" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:19">
@@ -5311,160 +5361,170 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:19"/>
+    <row r="72" spans="1:19">
+      <c r="B72" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="73" spans="1:19">
-      <c r="B73" s="4" t="s">
+      <c r="B73" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19"/>
+    <row r="75" spans="1:19">
+      <c r="B75" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C75" s="6" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19">
-      <c r="B74" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C74" s="16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19">
-      <c r="B75" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:19">
       <c r="B76" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:19">
       <c r="B77" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" s="16" t="s">
-        <v>127</v>
+        <v>71</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:19">
       <c r="B78" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:19">
       <c r="B79" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:19">
       <c r="B80" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:19">
       <c r="B81" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" spans="1:19">
       <c r="B82" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:19">
       <c r="B83" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:19">
       <c r="B84" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:19">
       <c r="B85" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:19">
       <c r="B86" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:19">
       <c r="B87" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:19">
       <c r="B88" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:19">
       <c r="B89" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:19">
       <c r="B90" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C90" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
+      <c r="B91" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C91" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
+      <c r="B92" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19">
-      <c r="B91" s="9" t="s">
+      <c r="C92" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19">
+      <c r="B93" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19"/>
+      <c r="C93" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -5494,18 +5554,18 @@
     <row r="2" spans="1:4"/>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4"/>
     <row r="5" spans="1:4">
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4"/>
@@ -5522,10 +5582,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="7" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>0</v>
@@ -5533,10 +5593,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="7" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>0</v>
@@ -5544,10 +5604,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="7" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>0</v>
@@ -5555,10 +5615,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="9" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>0</v>
@@ -5598,7 +5658,7 @@
     <row r="1" spans="1:2"/>
     <row r="2" spans="1:2">
       <c r="B2" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2"/>
@@ -5609,62 +5669,62 @@
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:2"/>
     <row r="7" spans="1:2">
       <c r="B7" s="13" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="18" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:2"/>
     <row r="10" spans="1:2">
       <c r="B10" s="13" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:2"/>
     <row r="13" spans="1:2">
       <c r="B13" s="13" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:2"/>
     <row r="16" spans="1:2">
       <c r="B16" s="13" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="B17" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:2"/>
     <row r="19" spans="1:2">
       <c r="B19" s="13" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow multiple settings for an inference tool
</commit_message>
<xml_diff>
--- a/germline_schema/docs/iarc_submission_sheet.xlsx
+++ b/germline_schema/docs/iarc_submission_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -512,6 +512,10 @@
   <si>
     <t>If multiple tools have been used, please create additional
 tables as needed.</t>
+  </si>
+  <si>
+    <t>If the same tool has been used with multiple settings (e.g. with different starting databases), please create a table for each setting used. 
+Please use a unique tool_name for each tool and setting combination, and use this name when referring to the tool in the Genotype table.</t>
   </si>
   <si>
     <t>tool_name</t>
@@ -5536,7 +5540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5545,7 +5549,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="2"/>
-    <col customWidth="1" max="2" min="2" width="60"/>
+    <col customWidth="1" max="2" min="2" width="143"/>
     <col customWidth="1" max="3" min="3" width="61"/>
     <col customWidth="1" max="4" min="4" width="50"/>
   </cols>
@@ -5568,35 +5572,29 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:4"/>
-    <row r="8" spans="1:4">
-      <c r="B8" s="4" t="s">
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4"/>
+    <row r="9" spans="1:4">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
         <v>141</v>
-      </c>
-      <c r="C10" t="s">
-        <v>142</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>0</v>
@@ -5604,33 +5602,44 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" t="s">
         <v>143</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4"/>
+      <c r="C13" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="14" spans="1:4"/>
     <row r="15" spans="1:4"/>
     <row r="16" spans="1:4"/>
     <row r="17" spans="1:4"/>
-    <row r="18" spans="1:4">
-      <c r="B18" s="1" t="n"/>
+    <row r="18" spans="1:4"/>
+    <row r="19" spans="1:4">
+      <c r="B19" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -5658,7 +5667,7 @@
     <row r="1" spans="1:2"/>
     <row r="2" spans="1:2">
       <c r="B2" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2"/>
@@ -5669,51 +5678,51 @@
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2"/>
     <row r="7" spans="1:2">
       <c r="B7" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:2"/>
     <row r="10" spans="1:2">
       <c r="B10" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:2"/>
     <row r="13" spans="1:2">
       <c r="B13" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:2"/>
     <row r="16" spans="1:2">
       <c r="B16" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="B17" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:2"/>
@@ -5724,7 +5733,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="B20" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>